<commit_message>
Added standalone grocery list test, fixed minor issues
</commit_message>
<xml_diff>
--- a/data_sources/scripts/files/FoodConnectsPeople.xlsx
+++ b/data_sources/scripts/files/FoodConnectsPeople.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Recipe" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11966" uniqueCount="1944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11964" uniqueCount="1944">
   <si>
     <t>id</t>
   </si>
@@ -13182,8 +13182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1166" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1182" sqref="F1182"/>
+    <sheetView topLeftCell="A1122" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1123" sqref="B1123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31339,6 +31339,9 @@
       <c r="C1123" s="1">
         <v>1</v>
       </c>
+      <c r="D1123" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="1124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1124" s="1">
@@ -32146,6 +32149,9 @@
       </c>
       <c r="D1182" s="1" t="s">
         <v>323</v>
+      </c>
+      <c r="F1182" s="1" t="s">
+        <v>1938</v>
       </c>
     </row>
     <row r="1183" spans="1:6" x14ac:dyDescent="0.25">
@@ -32198,10 +32204,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F392"/>
+  <dimension ref="A1:F391"/>
   <sheetViews>
-    <sheetView topLeftCell="A353" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A362" sqref="A362"/>
+    <sheetView tabSelected="1" topLeftCell="A265" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A284" sqref="A284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35100,19 +35106,13 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>1938</v>
+        <v>514</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="D225">
-        <v>15</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -35120,54 +35120,54 @@
         <v>514</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D226">
+        <v>5</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>514</v>
+        <v>535</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>332</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D227">
-        <v>5</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>28</v>
+        <v>332</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>535</v>
+        <v>569</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>332</v>
+        <v>458</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>332</v>
+        <v>458</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>569</v>
+        <v>584</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>458</v>
+        <v>328</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>458</v>
+        <v>328</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>584</v>
+        <v>130</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>328</v>
@@ -35178,7 +35178,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>130</v>
+        <v>68</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>328</v>
@@ -35192,55 +35192,55 @@
         <v>68</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>328</v>
+        <v>424</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D232">
+        <v>1000</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>424</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D233">
-        <v>1000</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>22</v>
+        <v>424</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>117</v>
+        <v>1921</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>424</v>
+        <v>323</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>424</v>
+        <v>328</v>
+      </c>
+      <c r="D234">
+        <v>10</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>1921</v>
+        <v>233</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="D235">
-        <v>10</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -35248,149 +35248,152 @@
         <v>233</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>328</v>
+        <v>424</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D236">
+        <v>1000</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>233</v>
+        <v>536</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>424</v>
+        <v>328</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D237">
-        <v>1000</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>536</v>
+        <v>545</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>545</v>
+        <v>481</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>323</v>
+        <v>471</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>323</v>
+        <v>471</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>471</v>
+      <c r="A240" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D240">
+        <v>0.3</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A241" s="2" t="s">
+      <c r="A241" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="B241" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C241" s="2" t="s">
+      <c r="B241" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="D241">
-        <v>0.3</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>22</v>
+      <c r="C241" s="1" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="B242" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="C242" s="1" t="s">
-        <v>332</v>
-      </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>391</v>
+        <v>91</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>91</v>
+        <v>344</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>328</v>
+        <v>424</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D244">
+        <v>1000</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
+      <c r="A245" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="B245" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C245" s="1" t="s">
+      <c r="B245" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C245" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D245">
-        <v>1000</v>
+        <v>150</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="B246" s="2" t="s">
+      <c r="A246" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B246" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C246" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D246">
-        <v>150</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>28</v>
+      <c r="C246" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>300</v>
+        <v>515</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>320</v>
+        <v>471</v>
+      </c>
+      <c r="D247">
+        <v>200</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -35398,40 +35401,37 @@
         <v>515</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>319</v>
+        <v>471</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D248">
-        <v>200</v>
-      </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>471</v>
+        <v>320</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>471</v>
+        <v>320</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>516</v>
+        <v>540</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>320</v>
+        <v>471</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>320</v>
+        <v>471</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>540</v>
+        <v>570</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>471</v>
@@ -35441,25 +35441,25 @@
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A252" s="1" t="s">
-        <v>570</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>471</v>
+      <c r="A252" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A253" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="B253" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="C253" s="2" t="s">
-        <v>332</v>
+      <c r="A253" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -35467,24 +35467,30 @@
         <v>582</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D254">
+        <v>20</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A255" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C255" s="1" t="s">
+      <c r="A255" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C255" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D255">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E255" s="1" t="s">
         <v>28</v>
@@ -35495,13 +35501,13 @@
         <v>327</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D256">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E256" s="1" t="s">
         <v>28</v>
@@ -35512,16 +35518,10 @@
         <v>327</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="D257">
-        <v>30</v>
-      </c>
-      <c r="E257" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -35529,24 +35529,30 @@
         <v>327</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>328</v>
       </c>
+      <c r="D258">
+        <v>10</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A259" s="2" t="s">
+      <c r="A259" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B259" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C259" s="2" t="s">
+      <c r="B259" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C259" s="1" t="s">
         <v>328</v>
       </c>
       <c r="D259">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E259" s="1" t="s">
         <v>28</v>
@@ -35556,78 +35562,72 @@
       <c r="A260" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B260" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C260" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D260">
-        <v>30</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>327</v>
+        <v>609</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>609</v>
+        <v>598</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>320</v>
+        <v>376</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
+      </c>
+      <c r="D262">
+        <v>200</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>598</v>
+        <v>565</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D263">
-        <v>200</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>28</v>
+        <v>332</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>565</v>
+        <v>600</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
+      </c>
+      <c r="D264">
+        <v>200</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>600</v>
+        <v>457</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="D265">
-        <v>200</v>
-      </c>
-      <c r="E265" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -35635,32 +35635,32 @@
         <v>457</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>328</v>
+        <v>458</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>328</v>
+        <v>458</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>457</v>
+        <v>505</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>458</v>
+        <v>320</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>458</v>
+        <v>320</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -35668,32 +35668,32 @@
         <v>508</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D269">
+        <v>20</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>508</v>
+        <v>445</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>323</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D270">
-        <v>20</v>
-      </c>
-      <c r="E270" s="1" t="s">
-        <v>28</v>
+        <v>323</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>323</v>
@@ -35704,100 +35704,100 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>450</v>
+        <v>361</v>
       </c>
       <c r="B272" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B273" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C272" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A273" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="B273" s="1" t="s">
+      <c r="C273" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="C273" s="1" t="s">
-        <v>471</v>
+      <c r="D273">
+        <v>30</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A274" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="B274" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C274" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="D274">
-        <v>30</v>
-      </c>
-      <c r="E274" s="1" t="s">
-        <v>22</v>
+      <c r="A274" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A275" s="1" t="s">
+      <c r="A275" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B275" s="1" t="s">
+      <c r="B275" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C275" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C275" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="D275">
+        <v>1000</v>
+      </c>
+      <c r="E275" s="1"/>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>424</v>
+        <v>320</v>
       </c>
       <c r="C276" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D276">
-        <v>1000</v>
-      </c>
-      <c r="E276" s="1"/>
+        <v>200</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A277" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B277" s="2" t="s">
+      <c r="A277" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B277" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C277" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D277">
-        <v>200</v>
-      </c>
-      <c r="E277" s="1" t="s">
-        <v>28</v>
+      <c r="C277" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>142</v>
+        <v>601</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>601</v>
+        <v>498</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>328</v>
@@ -35811,76 +35811,76 @@
         <v>498</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D280">
+        <v>10</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="B281" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="C281" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D281">
-        <v>10</v>
-      </c>
-      <c r="E281" s="1" t="s">
-        <v>28</v>
+        <v>447</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>447</v>
+        <v>1920</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D282">
+        <v>10</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>1920</v>
+        <v>359</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D283">
-        <v>10</v>
-      </c>
-      <c r="E283" s="1" t="s">
-        <v>28</v>
+        <v>320</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>359</v>
+        <v>578</v>
       </c>
       <c r="B284" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A285" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B285" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C284" s="1" t="s">
+      <c r="C285" s="2" t="s">
         <v>320</v>
-      </c>
-    </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A285" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="B285" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C285" s="1" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
-        <v>354</v>
+        <v>399</v>
       </c>
       <c r="B286" s="2" t="s">
         <v>320</v>
@@ -35891,27 +35891,33 @@
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
-        <v>399</v>
+        <v>597</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>320</v>
+        <v>471</v>
+      </c>
+      <c r="D287">
+        <v>200</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A288" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="B288" s="2" t="s">
+      <c r="A288" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B288" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="C288" s="2" t="s">
-        <v>471</v>
+      <c r="C288" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="D288">
         <v>200</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
@@ -35919,21 +35925,15 @@
         <v>97</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D289">
-        <v>200</v>
-      </c>
-      <c r="E289" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>97</v>
+        <v>1907</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>328</v>
@@ -35943,14 +35943,20 @@
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A291" s="1" t="s">
-        <v>1907</v>
-      </c>
-      <c r="B291" s="1" t="s">
+      <c r="A291" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C291" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C291" s="1" t="s">
-        <v>328</v>
+      <c r="D291">
+        <v>200</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -35958,21 +35964,15 @@
         <v>55</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C292" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D292">
-        <v>200</v>
-      </c>
-      <c r="E292" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>55</v>
+        <v>607</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>328</v>
@@ -35983,59 +35983,65 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="B294" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C294" s="2" t="s">
-        <v>328</v>
+        <v>382</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A295" s="2" t="s">
-        <v>382</v>
+      <c r="A295" s="1" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A296" s="1" t="s">
-        <v>537</v>
+      <c r="A296" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A297" s="2" t="s">
-        <v>637</v>
-      </c>
-      <c r="B297" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="C297" s="2" t="s">
-        <v>380</v>
+      <c r="A297" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>186</v>
+        <v>330</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>424</v>
+        <v>392</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>424</v>
+        <v>328</v>
+      </c>
+      <c r="D298">
+        <v>3</v>
+      </c>
+      <c r="E298" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A299" s="1" t="s">
+      <c r="A299" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B299" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="C299" s="1" t="s">
+      <c r="B299" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C299" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D299">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E299" s="1" t="s">
         <v>28</v>
@@ -36046,13 +36052,13 @@
         <v>330</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C300" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D300">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E300" s="1" t="s">
         <v>28</v>
@@ -36062,44 +36068,44 @@
       <c r="A301" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B301" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C301" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D301">
-        <v>15</v>
-      </c>
-      <c r="E301" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A302" s="2" t="s">
-        <v>330</v>
+      <c r="A302" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>579</v>
+        <v>606</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>424</v>
+        <v>328</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>424</v>
+        <v>328</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>606</v>
+        <v>470</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>328</v>
+        <v>320</v>
+      </c>
+      <c r="D304">
+        <v>5</v>
+      </c>
+      <c r="E304" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -36107,74 +36113,74 @@
         <v>470</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>341</v>
+        <v>320</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="D305">
-        <v>5</v>
-      </c>
-      <c r="E305" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A306" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="B306" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C306" s="1" t="s">
-        <v>320</v>
+      <c r="A306" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A307" s="2" t="s">
-        <v>402</v>
+      <c r="A307" s="1" t="s">
+        <v>571</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="B308" s="2" t="s">
+      <c r="B308" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C308" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C308" s="2" t="s">
+      <c r="D308">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A309" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A310" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C310" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A309" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="B309" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C309" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D309">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A310" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="B310" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="C310" s="2" t="s">
-        <v>332</v>
+      <c r="D310">
+        <v>30</v>
+      </c>
+      <c r="E310" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -36182,110 +36188,104 @@
         <v>432</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>328</v>
       </c>
       <c r="D311">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="E311" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A312" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="B312" s="1" t="s">
+      <c r="A312" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A313" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D313">
+        <v>1000</v>
+      </c>
+      <c r="E313" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A314" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B314" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C312" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D312">
-        <v>100</v>
-      </c>
-      <c r="E312" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A313" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B313" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C313" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A314" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B314" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C314" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D314">
-        <v>1000</v>
-      </c>
-      <c r="E314" s="1" t="s">
-        <v>22</v>
+      <c r="C314" s="2" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A315" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="B315" s="2" t="s">
+      <c r="A315" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B315" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C315" s="2" t="s">
+      <c r="C315" s="1" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>436</v>
+        <v>463</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>464</v>
+        <v>512</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>512</v>
+        <v>604</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>328</v>
@@ -36296,7 +36296,7 @@
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>604</v>
+        <v>454</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>328</v>
@@ -36306,93 +36306,99 @@
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A321" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="B321" s="1" t="s">
+      <c r="A321" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B321" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C321" s="1" t="s">
+      <c r="C321" s="2" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A322" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B322" s="2" t="s">
+      <c r="A322" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B322" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C322" s="2" t="s">
+      <c r="C322" s="1" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A323" s="1" t="s">
+      <c r="A323" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B323" s="1" t="s">
+      <c r="B323" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C323" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C323" s="1" t="s">
-        <v>328</v>
+      <c r="D323">
+        <v>50</v>
+      </c>
+      <c r="E323" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
-        <v>369</v>
+        <v>610</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>370</v>
+        <v>320</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D324">
-        <v>50</v>
-      </c>
-      <c r="E324" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="E324" s="1"/>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>610</v>
+        <v>331</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C325" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="E325" s="1"/>
+        <v>328</v>
+      </c>
+      <c r="D325">
+        <v>80</v>
+      </c>
+      <c r="E325" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A326" s="2" t="s">
+      <c r="A326" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B326" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C326" s="2" t="s">
+      <c r="B326" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D326">
-        <v>80</v>
-      </c>
-      <c r="E326" s="1" t="s">
-        <v>28</v>
+      <c r="C326" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A327" s="1" t="s">
+      <c r="A327" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B327" s="1" t="s">
+      <c r="B327" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C327" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C327" s="1" t="s">
-        <v>328</v>
+      <c r="D327">
+        <v>5</v>
+      </c>
+      <c r="E327" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
@@ -36400,74 +36406,68 @@
         <v>331</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C328" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D328">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E328" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A329" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="B329" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C329" s="2" t="s">
+      <c r="A329" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A330" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A331" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B331" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D329">
-        <v>15</v>
-      </c>
-      <c r="E329" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A330" s="1" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A331" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="B331" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="C331" s="2" t="s">
-        <v>332</v>
+      <c r="C331" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>473</v>
+        <v>622</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
+      </c>
+      <c r="D332">
+        <v>200</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>622</v>
+        <v>499</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D333">
-        <v>200</v>
+        <v>328</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -36475,38 +36475,44 @@
         <v>499</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C334" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D334">
+        <v>250</v>
+      </c>
+      <c r="E334" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="C335" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A336" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B336" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C336" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D335">
-        <v>250</v>
-      </c>
-      <c r="E335" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A336" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="B336" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="C336" s="1" t="s">
-        <v>332</v>
+      <c r="D336">
+        <v>150</v>
+      </c>
+      <c r="E336" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
@@ -36514,13 +36520,13 @@
         <v>366</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C337" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D337">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="E337" s="1" t="s">
         <v>28</v>
@@ -36528,131 +36534,128 @@
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>366</v>
+        <v>393</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C338" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D338">
-        <v>30</v>
-      </c>
-      <c r="E338" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A339" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="B339" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C339" s="2" t="s">
-        <v>328</v>
+      <c r="A339" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A340" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="B340" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C340" s="1" t="s">
-        <v>323</v>
+      <c r="A340" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="B340" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C340" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D340" t="s">
+        <v>441</v>
+      </c>
+      <c r="E340" s="2" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A341" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="B341" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C341" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="D341" t="s">
-        <v>441</v>
-      </c>
-      <c r="E341" s="2" t="s">
-        <v>441</v>
+      <c r="A341" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>625</v>
+        <v>483</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>518</v>
+        <v>323</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>518</v>
+        <v>323</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>483</v>
+        <v>44</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>323</v>
+        <v>424</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>323</v>
+        <v>328</v>
+      </c>
+      <c r="D343">
+        <v>1000</v>
+      </c>
+      <c r="E343" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A344" s="1" t="s">
+      <c r="A344" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B344" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C344" s="1" t="s">
+      <c r="B344" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C344" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D344">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="E344" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
-        <v>44</v>
+        <v>385</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C345" s="2" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
       <c r="D345">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="E345" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A346" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="B346" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C346" s="2" t="s">
+      <c r="A346" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C346" s="1" t="s">
         <v>471</v>
       </c>
       <c r="D346">
-        <v>30</v>
-      </c>
-      <c r="E346" s="1" t="s">
-        <v>22</v>
+        <v>400</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
@@ -36660,13 +36663,16 @@
         <v>564</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>530</v>
+        <v>328</v>
       </c>
       <c r="C347" s="1" t="s">
         <v>471</v>
       </c>
       <c r="D347">
-        <v>400</v>
+        <v>1</v>
+      </c>
+      <c r="E347" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
@@ -36674,60 +36680,54 @@
         <v>564</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
       <c r="C348" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D348">
-        <v>1</v>
-      </c>
-      <c r="E348" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>564</v>
+        <v>448</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>471</v>
+        <v>328</v>
       </c>
       <c r="C349" s="1" t="s">
         <v>471</v>
       </c>
+      <c r="D349">
+        <v>1</v>
+      </c>
+      <c r="E349" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A350" s="1" t="s">
+      <c r="A350" s="2" t="s">
         <v>448</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
       <c r="C350" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D350">
-        <v>1</v>
-      </c>
-      <c r="E350" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A351" s="2" t="s">
-        <v>448</v>
+      <c r="A351" s="1" t="s">
+        <v>533</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>471</v>
+        <v>328</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>471</v>
+        <v>328</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>328</v>
@@ -36741,127 +36741,133 @@
         <v>529</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>328</v>
+        <v>530</v>
       </c>
       <c r="C353" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D353">
+        <v>200</v>
+      </c>
+      <c r="E353" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>529</v>
+        <v>360</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>530</v>
+        <v>332</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D354">
-        <v>200</v>
-      </c>
-      <c r="E354" s="1" t="s">
-        <v>28</v>
+        <v>332</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A355" s="1" t="s">
+      <c r="A355" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B355" s="1" t="s">
+      <c r="B355" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C355" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C355" s="1" t="s">
-        <v>332</v>
+      <c r="D355">
+        <v>3</v>
+      </c>
+      <c r="E355" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
-        <v>360</v>
+        <v>375</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>323</v>
+        <v>376</v>
       </c>
       <c r="C356" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="D356">
-        <v>3</v>
-      </c>
-      <c r="E356" s="1" t="s">
-        <v>22</v>
+        <v>376</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A357" s="2" t="s">
-        <v>375</v>
+      <c r="A357" s="1" t="s">
+        <v>630</v>
       </c>
       <c r="B357" s="2" t="s">
-        <v>376</v>
+        <v>328</v>
       </c>
       <c r="C357" s="2" t="s">
-        <v>376</v>
+        <v>328</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="B358" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C358" s="2" t="s">
-        <v>328</v>
+        <v>547</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A359" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="B359" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C359" s="1" t="s">
-        <v>320</v>
+      <c r="A359" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B359" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A360" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="B360" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="C360" s="2" t="s">
-        <v>409</v>
+      <c r="A360" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>593</v>
+        <v>1936</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>594</v>
+        <v>323</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>594</v>
+        <v>328</v>
+      </c>
+      <c r="D361">
+        <v>15</v>
+      </c>
+      <c r="E361" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>1936</v>
+        <v>501</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>323</v>
+        <v>518</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
       <c r="D362">
-        <v>15</v>
+        <v>1000</v>
       </c>
       <c r="E362" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
@@ -36869,41 +36875,41 @@
         <v>501</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>518</v>
+        <v>471</v>
       </c>
       <c r="C363" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D363">
-        <v>1000</v>
-      </c>
-      <c r="E363" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>501</v>
+        <v>1908</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>471</v>
+        <v>323</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>471</v>
+        <v>328</v>
+      </c>
+      <c r="D364">
+        <v>30</v>
+      </c>
+      <c r="E364" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A365" s="1" t="s">
-        <v>1908</v>
-      </c>
-      <c r="B365" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C365" s="1" t="s">
+      <c r="A365" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B365" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C365" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D365">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E365" s="1" t="s">
         <v>28</v>
@@ -36914,16 +36920,10 @@
         <v>345</v>
       </c>
       <c r="B366" s="2" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="D366">
-        <v>50</v>
-      </c>
-      <c r="E366" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
@@ -36931,20 +36931,26 @@
         <v>345</v>
       </c>
       <c r="B367" s="2" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>328</v>
       </c>
+      <c r="D367">
+        <v>10</v>
+      </c>
+      <c r="E367" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A368" s="2" t="s">
+      <c r="A368" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B368" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C368" s="2" t="s">
+      <c r="B368" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C368" s="1" t="s">
         <v>328</v>
       </c>
       <c r="D368">
@@ -36955,37 +36961,37 @@
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A369" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="B369" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C369" s="1" t="s">
-        <v>328</v>
+      <c r="A369" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B369" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>471</v>
       </c>
       <c r="D369">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="E369" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A370" s="2" t="s">
+      <c r="A370" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B370" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C370" s="2" t="s">
+      <c r="B370" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C370" s="1" t="s">
         <v>471</v>
       </c>
       <c r="D370">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="E370" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
@@ -36993,16 +36999,10 @@
         <v>377</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>518</v>
+        <v>471</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="D371">
-        <v>1000</v>
-      </c>
-      <c r="E371" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -37010,53 +37010,59 @@
         <v>377</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>471</v>
+        <v>323</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>471</v>
       </c>
+      <c r="D372">
+        <v>30</v>
+      </c>
+      <c r="E372" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>377</v>
+        <v>1881</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D373">
-        <v>30</v>
-      </c>
-      <c r="E373" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="E373" s="1"/>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>1881</v>
+        <v>1922</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>328</v>
+        <v>1923</v>
       </c>
       <c r="C374" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="E374" s="1"/>
+      <c r="D374">
+        <v>200</v>
+      </c>
+      <c r="E374" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>1922</v>
+        <v>603</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>1923</v>
+        <v>320</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>328</v>
       </c>
       <c r="D375">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E375" s="1" t="s">
         <v>28</v>
@@ -37064,33 +37070,33 @@
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>603</v>
+        <v>404</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="C376" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
       <c r="D376">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E376" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A377" s="1" t="s">
+      <c r="A377" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B377" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="C377" s="1" t="s">
+      <c r="B377" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C377" s="2" t="s">
         <v>471</v>
       </c>
       <c r="D377">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E377" s="1" t="s">
         <v>22</v>
@@ -37098,45 +37104,45 @@
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
-        <v>404</v>
+        <v>538</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>471</v>
       </c>
       <c r="D378">
-        <v>30</v>
-      </c>
-      <c r="E378" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="E378" s="1"/>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A379" s="2" t="s">
+      <c r="A379" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="B379" s="2" t="s">
+      <c r="B379" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A380" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B380" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="C379" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="D379">
+      <c r="C380" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D380">
         <v>200</v>
       </c>
-      <c r="E379" s="1"/>
-    </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A380" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="B380" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="C380" s="1" t="s">
-        <v>471</v>
+      <c r="E380" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.25">
@@ -37144,49 +37150,43 @@
         <v>338</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D381">
-        <v>200</v>
-      </c>
-      <c r="E381" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A382" s="2" t="s">
+      <c r="A382" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B382" s="2" t="s">
+      <c r="B382" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C382" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C382" s="2" t="s">
+      <c r="D382">
+        <v>30</v>
+      </c>
+      <c r="E382" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A383" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A384" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B384" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A383" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B383" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C383" s="1" t="s">
+      <c r="C384" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="D383">
-        <v>30</v>
-      </c>
-      <c r="E383" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A384" s="2" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.25">
@@ -37194,27 +37194,33 @@
         <v>414</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C385" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D385">
+        <v>20</v>
+      </c>
+      <c r="E385" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>414</v>
+        <v>517</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>323</v>
+        <v>518</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
       <c r="D386">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="E386" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
@@ -37222,70 +37228,53 @@
         <v>517</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>518</v>
+        <v>471</v>
       </c>
       <c r="C387" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D387">
-        <v>1000</v>
-      </c>
-      <c r="E387" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>517</v>
+        <v>628</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>471</v>
+        <v>328</v>
       </c>
       <c r="C388" s="1" t="s">
-        <v>471</v>
+        <v>328</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>328</v>
+        <v>594</v>
       </c>
       <c r="C389" s="1" t="s">
-        <v>328</v>
+        <v>594</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>595</v>
+        <v>401</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>594</v>
+        <v>320</v>
       </c>
       <c r="C390" s="1" t="s">
-        <v>594</v>
+        <v>320</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A391" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="B391" s="1" t="s">
+      <c r="A391" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B391" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C391" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A392" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B392" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C392" s="2" t="s">
+      <c r="C391" s="2" t="s">
         <v>320</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added pastitsio recipe from Kalamata
</commit_message>
<xml_diff>
--- a/data_sources/scripts/files/FoodConnectsPeople.xlsx
+++ b/data_sources/scripts/files/FoodConnectsPeople.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Recipe" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11964" uniqueCount="1944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12034" uniqueCount="1953">
   <si>
     <t>id</t>
   </si>
@@ -5868,6 +5868,33 @@
   </si>
   <si>
     <t>burro vegano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pastitsio (baked pasta with minced beef) </t>
+  </si>
+  <si>
+    <t>recipes/mediterranea/greece/pastitsio-baked-pasta-with-minced-beef</t>
+  </si>
+  <si>
+    <t>pasta; beef meat</t>
+  </si>
+  <si>
+    <t>Pasticcio di pasta e carne</t>
+  </si>
+  <si>
+    <t>it/ricette/paesi-mediterranei/grecia/pasticcio-di-pasta-e-carne</t>
+  </si>
+  <si>
+    <t>spaghetti</t>
+  </si>
+  <si>
+    <t>soy strip</t>
+  </si>
+  <si>
+    <t>pasta; carne di manzo</t>
+  </si>
+  <si>
+    <t>carne di soia</t>
   </si>
 </sst>
 </file>
@@ -5878,7 +5905,7 @@
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5907,6 +5934,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -5929,7 +5962,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -5965,6 +5998,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -6248,10 +6284,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P105"/>
+  <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView topLeftCell="D94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K106" sqref="K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10898,6 +10934,50 @@
       </c>
       <c r="P105" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>1944</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>1945</v>
+      </c>
+      <c r="D106" s="1">
+        <v>70</v>
+      </c>
+      <c r="E106" s="1">
+        <v>6</v>
+      </c>
+      <c r="F106" s="1">
+        <v>4</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>1946</v>
+      </c>
+      <c r="L106" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M106" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N106" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O106" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P106" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -11283,7 +11363,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
     <sheetView topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C106" sqref="C106"/>
@@ -12765,6 +12845,20 @@
       </c>
       <c r="D105" s="1" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>99</v>
+      </c>
+      <c r="B106" s="1">
+        <v>105</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>1944</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -13180,10 +13274,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1185"/>
+  <dimension ref="A1:G1198"/>
   <sheetViews>
-    <sheetView topLeftCell="A1122" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1123" sqref="B1123"/>
+    <sheetView topLeftCell="A1181" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1195" sqref="B1195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32182,7 +32276,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="1185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1185" s="1">
         <v>104</v>
       </c>
@@ -32194,6 +32288,167 @@
       </c>
       <c r="D1185" s="1" t="s">
         <v>320</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1186" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1186" s="13" t="s">
+        <v>1949</v>
+      </c>
+      <c r="C1186" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1186" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1187" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1187" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1187" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1187" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1188" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1188" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1188" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1188" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E1188" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="F1188" s="1" t="s">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1189" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1189" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="C1189" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1189" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E1189" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1190" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1190" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1190" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1190" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1191" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1191" s="13" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1192" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1192" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="C1192" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D1192" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1193" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1193" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1193" s="1">
+        <v>150</v>
+      </c>
+      <c r="D1193" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1194" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1194" s="13" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1195" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1195" s="13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1196" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1196" s="13" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1197" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1197" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1198" s="1">
+        <v>105</v>
+      </c>
+      <c r="B1198" s="13" t="s">
+        <v>597</v>
+      </c>
+      <c r="C1198" s="1">
+        <v>100</v>
+      </c>
+      <c r="D1198" s="1" t="s">
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -32204,10 +32459,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F391"/>
+  <dimension ref="A1:F393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A284" sqref="A284"/>
+    <sheetView topLeftCell="A306" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A320" sqref="A320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35894,30 +36149,24 @@
         <v>597</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>319</v>
+        <v>471</v>
       </c>
       <c r="C287" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="D287">
-        <v>200</v>
-      </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A288" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B288" s="1" t="s">
+      <c r="A288" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="B288" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="C288" s="1" t="s">
-        <v>328</v>
+      <c r="C288" s="2" t="s">
+        <v>471</v>
       </c>
       <c r="D288">
         <v>200</v>
-      </c>
-      <c r="E288" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
@@ -35925,15 +36174,21 @@
         <v>97</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D289">
+        <v>200</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>1907</v>
+        <v>97</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>328</v>
@@ -35943,20 +36198,14 @@
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A291" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B291" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C291" s="2" t="s">
+      <c r="A291" s="1" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B291" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D291">
-        <v>200</v>
-      </c>
-      <c r="E291" s="1" t="s">
-        <v>28</v>
+      <c r="C291" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -35964,15 +36213,21 @@
         <v>55</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C292" s="2" t="s">
         <v>328</v>
       </c>
+      <c r="D292">
+        <v>200</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>607</v>
+        <v>55</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>328</v>
@@ -35983,65 +36238,59 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A295" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A295" s="1" t="s">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A296" s="1" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A296" s="2" t="s">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A297" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="B296" s="2" t="s">
+      <c r="B297" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="C296" s="2" t="s">
+      <c r="C297" s="2" t="s">
         <v>380</v>
-      </c>
-    </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A297" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B297" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C297" s="1" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A299" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B298" s="1" t="s">
+      <c r="B299" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="C298" s="1" t="s">
+      <c r="C299" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D298">
+      <c r="D299">
         <v>3</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A299" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="B299" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="C299" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D299">
-        <v>5</v>
       </c>
       <c r="E299" s="1" t="s">
         <v>28</v>
@@ -36052,13 +36301,13 @@
         <v>330</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="C300" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D300">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E300" s="1" t="s">
         <v>28</v>
@@ -36068,44 +36317,44 @@
       <c r="A301" s="2" t="s">
         <v>330</v>
       </c>
+      <c r="B301" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D301">
+        <v>15</v>
+      </c>
+      <c r="E301" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A302" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="B302" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C302" s="1" t="s">
-        <v>424</v>
+      <c r="A302" s="2" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>606</v>
+        <v>579</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>328</v>
+        <v>424</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>328</v>
+        <v>424</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>470</v>
+        <v>606</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D304">
-        <v>5</v>
-      </c>
-      <c r="E304" s="1" t="s">
-        <v>28</v>
+        <v>328</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -36113,74 +36362,74 @@
         <v>470</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>320</v>
+        <v>341</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>320</v>
       </c>
+      <c r="D305">
+        <v>5</v>
+      </c>
+      <c r="E305" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A306" s="2" t="s">
+      <c r="A306" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A307" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B306" s="2" t="s">
+      <c r="B307" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C306" s="2" t="s">
+      <c r="C307" s="2" t="s">
         <v>323</v>
-      </c>
-    </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A307" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="B307" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C307" s="2" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="B308" s="1" t="s">
+      <c r="B308" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A309" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B309" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C308" s="1" t="s">
+      <c r="C309" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D308">
+      <c r="D309">
         <v>1000</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A309" s="2" t="s">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A310" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B309" s="2" t="s">
+      <c r="B310" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C309" s="2" t="s">
+      <c r="C310" s="2" t="s">
         <v>332</v>
-      </c>
-    </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A310" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="B310" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C310" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D310">
-        <v>30</v>
-      </c>
-      <c r="E310" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -36188,104 +36437,110 @@
         <v>432</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>328</v>
       </c>
       <c r="D311">
+        <v>30</v>
+      </c>
+      <c r="E311" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A312" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D312">
         <v>100</v>
       </c>
-      <c r="E311" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A312" s="2" t="s">
+      <c r="E312" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A313" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B312" s="2" t="s">
+      <c r="B313" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C312" s="2" t="s">
+      <c r="C313" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A313" s="1" t="s">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A314" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B313" s="1" t="s">
+      <c r="B314" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C313" s="1" t="s">
+      <c r="C314" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D313">
+      <c r="D314">
         <v>1000</v>
       </c>
-      <c r="E313" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A314" s="2" t="s">
+      <c r="E314" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A315" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B314" s="2" t="s">
+      <c r="B315" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C314" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A315" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="B315" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C315" s="1" t="s">
+      <c r="C315" s="2" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>512</v>
+        <v>464</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>604</v>
+        <v>512</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>328</v>
@@ -36296,29 +36551,35 @@
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>454</v>
+        <v>1949</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>328</v>
+        <v>424</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D320">
+        <v>1000</v>
+      </c>
+      <c r="E320" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A321" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B321" s="2" t="s">
+      <c r="A321" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B321" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C321" s="2" t="s">
+      <c r="C321" s="1" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>369</v>
+        <v>454</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>328</v>
@@ -36329,139 +36590,136 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
-        <v>369</v>
+        <v>60</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>370</v>
+        <v>328</v>
       </c>
       <c r="C323" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D323">
-        <v>50</v>
-      </c>
-      <c r="E323" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A324" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="B324" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C324" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="E324" s="1"/>
+      <c r="A324" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>331</v>
+        <v>369</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>319</v>
+        <v>370</v>
       </c>
       <c r="C325" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D325">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E325" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A326" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="B326" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C326" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="A326" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E326" s="1"/>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
         <v>331</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="C327" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D327">
+        <v>80</v>
+      </c>
+      <c r="E327" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A328" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A329" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D329">
         <v>5</v>
       </c>
-      <c r="E327" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A328" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="B328" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C328" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D328">
-        <v>15</v>
-      </c>
-      <c r="E328" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A329" s="1" t="s">
-        <v>546</v>
+      <c r="E329" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
-        <v>356</v>
+        <v>331</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
+      </c>
+      <c r="D330">
+        <v>15</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="B331" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C331" s="1" t="s">
-        <v>328</v>
+        <v>546</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A332" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="B332" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="C332" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D332">
-        <v>200</v>
+      <c r="A332" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C332" s="2" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>499</v>
+        <v>473</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>328</v>
@@ -36472,207 +36730,201 @@
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>499</v>
+        <v>622</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
       <c r="D334">
-        <v>250</v>
-      </c>
-      <c r="E334" s="1" t="s">
-        <v>28</v>
+        <v>200</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A336" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D336">
+        <v>250</v>
+      </c>
+      <c r="E336" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="B335" s="1" t="s">
+      <c r="B337" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C335" s="1" t="s">
+      <c r="C337" s="1" t="s">
         <v>332</v>
-      </c>
-    </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A336" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="B336" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C336" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D336">
-        <v>150</v>
-      </c>
-      <c r="E336" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A337" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="B337" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C337" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D337">
-        <v>30</v>
-      </c>
-      <c r="E337" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>393</v>
+        <v>366</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C338" s="2" t="s">
         <v>328</v>
       </c>
+      <c r="D338">
+        <v>150</v>
+      </c>
+      <c r="E338" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A339" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="B339" s="1" t="s">
+      <c r="A339" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B339" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C339" s="1" t="s">
-        <v>323</v>
+      <c r="C339" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D339">
+        <v>30</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
-        <v>633</v>
+        <v>393</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C340" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="D340" t="s">
-        <v>441</v>
-      </c>
-      <c r="E340" s="2" t="s">
-        <v>441</v>
+        <v>328</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>625</v>
+        <v>552</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>518</v>
+        <v>323</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>518</v>
+        <v>323</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A342" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="B342" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C342" s="1" t="s">
-        <v>323</v>
+      <c r="A342" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="B342" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C342" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D342" t="s">
+        <v>441</v>
+      </c>
+      <c r="E342" s="2" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A344" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A345" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B343" s="1" t="s">
+      <c r="B345" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C343" s="1" t="s">
+      <c r="C345" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D343">
+      <c r="D345">
         <v>1000</v>
       </c>
-      <c r="E343" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A344" s="2" t="s">
+      <c r="E345" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A346" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B344" s="2" t="s">
+      <c r="B346" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C344" s="2" t="s">
+      <c r="C346" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D344">
+      <c r="D346">
         <v>100</v>
       </c>
-      <c r="E344" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A345" s="2" t="s">
+      <c r="E346" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A347" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B345" s="2" t="s">
+      <c r="B347" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C345" s="2" t="s">
+      <c r="C347" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="D345">
+      <c r="D347">
         <v>30</v>
       </c>
-      <c r="E345" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A346" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="B346" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="C346" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D346">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A347" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="B347" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C347" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D347">
-        <v>1</v>
-      </c>
       <c r="E347" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
@@ -36680,15 +36932,18 @@
         <v>564</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>471</v>
+        <v>530</v>
       </c>
       <c r="C348" s="1" t="s">
         <v>471</v>
       </c>
+      <c r="D348">
+        <v>400</v>
+      </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>448</v>
+        <v>564</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>328</v>
@@ -36704,8 +36959,8 @@
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A350" s="2" t="s">
-        <v>448</v>
+      <c r="A350" s="1" t="s">
+        <v>564</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>471</v>
@@ -36716,214 +36971,214 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
-        <v>533</v>
+        <v>448</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>328</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
+      </c>
+      <c r="D351">
+        <v>1</v>
+      </c>
+      <c r="E351" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A352" s="1" t="s">
-        <v>529</v>
+      <c r="A352" s="2" t="s">
+        <v>448</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>530</v>
+        <v>328</v>
       </c>
       <c r="C353" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D353">
-        <v>200</v>
-      </c>
-      <c r="E353" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A355" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D355">
+        <v>200</v>
+      </c>
+      <c r="E355" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A356" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B354" s="1" t="s">
+      <c r="B356" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C354" s="1" t="s">
+      <c r="C356" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A355" s="2" t="s">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A357" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B355" s="2" t="s">
+      <c r="B357" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C355" s="2" t="s">
+      <c r="C357" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="D355">
+      <c r="D357">
         <v>3</v>
       </c>
-      <c r="E355" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A356" s="2" t="s">
+      <c r="E357" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A358" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B356" s="2" t="s">
+      <c r="B358" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="C356" s="2" t="s">
+      <c r="C358" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A357" s="1" t="s">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="B357" s="2" t="s">
+      <c r="B359" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C357" s="2" t="s">
+      <c r="C359" s="2" t="s">
         <v>328</v>
-      </c>
-    </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A358" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="B358" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C358" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A359" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="B359" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="C359" s="2" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>593</v>
+        <v>547</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>594</v>
+        <v>320</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>594</v>
+        <v>320</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A361" s="1" t="s">
-        <v>1936</v>
-      </c>
-      <c r="B361" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C361" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D361">
-        <v>15</v>
-      </c>
-      <c r="E361" s="1" t="s">
-        <v>28</v>
+      <c r="A361" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B361" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>501</v>
+        <v>593</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>518</v>
+        <v>594</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D362">
-        <v>1000</v>
-      </c>
-      <c r="E362" s="1" t="s">
-        <v>22</v>
+        <v>594</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>501</v>
+        <v>1936</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>471</v>
+        <v>323</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>471</v>
+        <v>328</v>
+      </c>
+      <c r="D363">
+        <v>15</v>
+      </c>
+      <c r="E363" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D364">
+        <v>1000</v>
+      </c>
+      <c r="E364" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A365" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A366" s="1" t="s">
         <v>1908</v>
       </c>
-      <c r="B364" s="1" t="s">
+      <c r="B366" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C364" s="1" t="s">
+      <c r="C366" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D364">
+      <c r="D366">
         <v>30</v>
       </c>
-      <c r="E364" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A365" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="B365" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C365" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D365">
-        <v>50</v>
-      </c>
-      <c r="E365" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A366" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="B366" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C366" s="2" t="s">
-        <v>328</v>
+      <c r="E366" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
@@ -36931,47 +37186,41 @@
         <v>345</v>
       </c>
       <c r="B367" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D367">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E367" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A368" s="1" t="s">
+      <c r="A368" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B368" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C368" s="1" t="s">
+      <c r="B368" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D368">
-        <v>10</v>
-      </c>
-      <c r="E368" s="1" t="s">
-        <v>28</v>
+      <c r="C368" s="2" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>377</v>
+        <v>345</v>
       </c>
       <c r="B369" s="2" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C369" s="2" t="s">
-        <v>471</v>
+        <v>328</v>
       </c>
       <c r="D369">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="E369" s="1" t="s">
         <v>28</v>
@@ -36979,30 +37228,36 @@
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D370">
+        <v>10</v>
+      </c>
+      <c r="E370" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A371" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B370" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="C370" s="1" t="s">
+      <c r="B371" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C371" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="D370">
-        <v>1000</v>
-      </c>
-      <c r="E370" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A371" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="B371" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="C371" s="1" t="s">
-        <v>471</v>
+      <c r="D371">
+        <v>200</v>
+      </c>
+      <c r="E371" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -37010,13 +37265,13 @@
         <v>377</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>323</v>
+        <v>518</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>471</v>
       </c>
       <c r="D372">
-        <v>30</v>
+        <v>1000</v>
       </c>
       <c r="E372" s="1" t="s">
         <v>22</v>
@@ -37024,150 +37279,150 @@
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>1881</v>
+        <v>377</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="E373" s="1"/>
+        <v>471</v>
+      </c>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>1922</v>
+        <v>377</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>1923</v>
+        <v>323</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
       <c r="D374">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="E374" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>603</v>
+        <v>1881</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D375">
-        <v>100</v>
-      </c>
-      <c r="E375" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="E375" s="1"/>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>1923</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D376">
+        <v>200</v>
+      </c>
+      <c r="E376" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A377" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D377">
+        <v>100</v>
+      </c>
+      <c r="E377" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A378" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="B376" s="1" t="s">
+      <c r="B378" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C376" s="1" t="s">
+      <c r="C378" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D376">
+      <c r="D378">
         <v>10</v>
       </c>
-      <c r="E376" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A377" s="2" t="s">
+      <c r="E378" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A379" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B377" s="2" t="s">
+      <c r="B379" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C377" s="2" t="s">
+      <c r="C379" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="D377">
+      <c r="D379">
         <v>30</v>
       </c>
-      <c r="E377" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A378" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="B378" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C378" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="D378">
-        <v>200</v>
-      </c>
-      <c r="E378" s="1"/>
-    </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A379" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="B379" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="C379" s="1" t="s">
-        <v>471</v>
+      <c r="E379" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>338</v>
+        <v>538</v>
       </c>
       <c r="B380" s="2" t="s">
         <v>319</v>
       </c>
       <c r="C380" s="2" t="s">
-        <v>328</v>
+        <v>471</v>
       </c>
       <c r="D380">
         <v>200</v>
       </c>
-      <c r="E380" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="E380" s="1"/>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A381" s="2" t="s">
+      <c r="A381" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A382" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B381" s="2" t="s">
+      <c r="B382" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C382" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C381" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A382" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B382" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C382" s="1" t="s">
-        <v>328</v>
-      </c>
       <c r="D382">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="E382" s="1" t="s">
         <v>28</v>
@@ -37177,104 +37432,132 @@
       <c r="A383" s="2" t="s">
         <v>338</v>
       </c>
+      <c r="B383" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C383" s="2" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
-        <v>414</v>
+        <v>338</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C384" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D384">
+        <v>30</v>
+      </c>
+      <c r="E384" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A385" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="B385" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C385" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D385">
-        <v>20</v>
-      </c>
-      <c r="E385" s="1" t="s">
-        <v>28</v>
+      <c r="A385" s="2" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>517</v>
+        <v>414</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>518</v>
+        <v>328</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D386">
-        <v>1000</v>
-      </c>
-      <c r="E386" s="1" t="s">
-        <v>22</v>
+        <v>328</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>517</v>
+        <v>414</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>471</v>
+        <v>323</v>
       </c>
       <c r="C387" s="1" t="s">
-        <v>471</v>
+        <v>328</v>
+      </c>
+      <c r="D387">
+        <v>20</v>
+      </c>
+      <c r="E387" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>628</v>
+        <v>517</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>328</v>
+        <v>518</v>
       </c>
       <c r="C388" s="1" t="s">
-        <v>328</v>
+        <v>471</v>
+      </c>
+      <c r="D388">
+        <v>1000</v>
+      </c>
+      <c r="E388" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>595</v>
+        <v>517</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>594</v>
+        <v>471</v>
       </c>
       <c r="C389" s="1" t="s">
-        <v>594</v>
+        <v>471</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A391" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A392" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="B390" s="1" t="s">
+      <c r="B392" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C390" s="1" t="s">
+      <c r="C392" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A391" s="2" t="s">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A393" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B391" s="2" t="s">
+      <c r="B393" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C391" s="2" t="s">
+      <c r="C393" s="2" t="s">
         <v>320</v>
       </c>
     </row>
@@ -37488,10 +37771,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B109"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
     <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38371,6 +38654,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>105</v>
+      </c>
+      <c r="B110">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -38379,10 +38670,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C254"/>
+  <dimension ref="A1:C257"/>
   <sheetViews>
-    <sheetView topLeftCell="A239" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A255" sqref="A255"/>
+    <sheetView topLeftCell="A238" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A257" sqref="A257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41167,6 +41458,39 @@
         <v>1</v>
       </c>
     </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
+        <v>105</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="C255" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
+        <v>105</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="C256" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" s="1">
+        <v>105</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="C257" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -41175,10 +41499,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G282"/>
+  <dimension ref="A1:G284"/>
   <sheetViews>
-    <sheetView topLeftCell="A257" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A265" sqref="A265"/>
+    <sheetView tabSelected="1" topLeftCell="A221" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A231" sqref="A231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46479,7 +46803,7 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>464</v>
+        <v>1950</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>22</v>
@@ -46502,7 +46826,7 @@
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>512</v>
+        <v>464</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>22</v>
@@ -46520,18 +46844,18 @@
         <v>28</v>
       </c>
       <c r="G232" s="1" t="s">
-        <v>715</v>
+        <v>726</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>604</v>
+        <v>512</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D233" s="1" t="s">
         <v>22</v>
@@ -46543,81 +46867,81 @@
         <v>28</v>
       </c>
       <c r="G233" s="1" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G234" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G235" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B234" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C234" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D234" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F234" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G234" s="1" t="s">
+      <c r="B236" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G236" s="1" t="s">
         <v>728</v>
-      </c>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A235" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C235" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D235" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F235" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G235" s="1" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A236" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F236" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G236" s="1" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>610</v>
+        <v>60</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>22</v>
@@ -46632,15 +46956,15 @@
         <v>22</v>
       </c>
       <c r="F237" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>715</v>
+        <v>720</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>331</v>
+        <v>369</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>22</v>
@@ -46649,7 +46973,7 @@
         <v>22</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E238" s="1" t="s">
         <v>22</v>
@@ -46658,12 +46982,12 @@
         <v>28</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
-        <v>546</v>
+      <c r="A239" s="2" t="s">
+        <v>610</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>22</v>
@@ -46678,15 +47002,15 @@
         <v>22</v>
       </c>
       <c r="F239" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G239" s="1" t="s">
-        <v>725</v>
+        <v>715</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>356</v>
+        <v>331</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>22</v>
@@ -46701,15 +47025,15 @@
         <v>22</v>
       </c>
       <c r="F240" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G240" s="1" t="s">
-        <v>715</v>
+        <v>725</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>473</v>
+        <v>546</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>22</v>
@@ -46727,12 +47051,12 @@
         <v>28</v>
       </c>
       <c r="G241" s="1" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A242" s="1" t="s">
-        <v>622</v>
+      <c r="A242" s="2" t="s">
+        <v>356</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>22</v>
@@ -46747,15 +47071,15 @@
         <v>22</v>
       </c>
       <c r="F242" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>499</v>
+        <v>473</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>22</v>
@@ -46778,7 +47102,7 @@
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>509</v>
+        <v>622</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>22</v>
@@ -46801,122 +47125,122 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G245" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G246" s="1" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="B245" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C245" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D245" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E245" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F245" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G245" s="1" t="s">
+      <c r="B247" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G247" s="1" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B246" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C246" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D246" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F246" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G246" s="1" t="s">
+      <c r="B248" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G248" s="1" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A247" s="2" t="s">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B247" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C247" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D247" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F247" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G247" s="1" t="s">
+      <c r="B249" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G249" s="1" t="s">
         <v>721</v>
-      </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A248" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C248" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D248" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F248" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G248" s="1" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="B249" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C249" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D249" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F249" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G249" s="1" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>625</v>
+        <v>552</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>22</v>
@@ -46934,104 +47258,104 @@
         <v>28</v>
       </c>
       <c r="G250" s="1" t="s">
-        <v>732</v>
+        <v>715</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G251" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F252" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G252" s="1" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="B251" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C251" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D251" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F251" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G251" s="1" t="s">
+      <c r="B253" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G253" s="1" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A252" s="2" t="s">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B252" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D252" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E252" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F252" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G252" s="1" t="s">
+      <c r="B254" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G254" s="1" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253" s="2" t="s">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
         <v>385</v>
-      </c>
-      <c r="B253" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C253" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D253" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E253" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F253" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G253" s="1" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A254" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="B254" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D254" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F254" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G254" s="1" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A255" s="1" t="s">
-        <v>448</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>22</v>
@@ -47054,36 +47378,36 @@
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>533</v>
+        <v>564</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D256" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F256" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G256" s="1" t="s">
-        <v>721</v>
+        <v>726</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>529</v>
+        <v>448</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D257" s="1" t="s">
         <v>22</v>
@@ -47099,37 +47423,37 @@
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A258" s="2" t="s">
-        <v>360</v>
+      <c r="A258" s="1" t="s">
+        <v>533</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D258" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F258" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G258" s="1" t="s">
-        <v>715</v>
+        <v>721</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A259" s="2" t="s">
-        <v>375</v>
+      <c r="A259" s="1" t="s">
+        <v>529</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D259" s="1" t="s">
         <v>22</v>
@@ -47141,12 +47465,12 @@
         <v>28</v>
       </c>
       <c r="G259" s="1" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>497</v>
+        <v>360</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>22</v>
@@ -47168,31 +47492,31 @@
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A261" s="1" t="s">
-        <v>630</v>
+      <c r="A261" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="B261" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D261" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F261" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G261" s="1" t="s">
-        <v>721</v>
+        <v>731</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
-        <v>547</v>
+      <c r="A262" s="2" t="s">
+        <v>497</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>22</v>
@@ -47214,31 +47538,31 @@
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A263" s="2" t="s">
-        <v>408</v>
+      <c r="A263" s="1" t="s">
+        <v>630</v>
       </c>
       <c r="B263" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D263" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F263" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>593</v>
+        <v>547</v>
       </c>
       <c r="B264" s="1" t="s">
         <v>22</v>
@@ -47253,38 +47577,38 @@
         <v>22</v>
       </c>
       <c r="F264" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G264" s="1" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F265" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G265" s="1" t="s">
         <v>722</v>
-      </c>
-    </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A265" s="1" t="s">
-        <v>1936</v>
-      </c>
-      <c r="B265" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C265" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D265" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E265" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F265" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G265" s="1" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>501</v>
+        <v>593</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>22</v>
@@ -47299,15 +47623,15 @@
         <v>22</v>
       </c>
       <c r="F266" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G266" s="1" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>583</v>
+        <v>1936</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>22</v>
@@ -47325,18 +47649,18 @@
         <v>28</v>
       </c>
       <c r="G267" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>1908</v>
+        <v>501</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D268" s="1" t="s">
         <v>22</v>
@@ -47352,8 +47676,8 @@
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A269" s="2" t="s">
-        <v>345</v>
+      <c r="A269" s="1" t="s">
+        <v>583</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>22</v>
@@ -47371,18 +47695,18 @@
         <v>28</v>
       </c>
       <c r="G269" s="1" t="s">
-        <v>716</v>
+        <v>722</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A270" s="2" t="s">
-        <v>377</v>
+      <c r="A270" s="1" t="s">
+        <v>1908</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D270" s="1" t="s">
         <v>22</v>
@@ -47394,12 +47718,12 @@
         <v>28</v>
       </c>
       <c r="G270" s="1" t="s">
-        <v>377</v>
+        <v>726</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>1881</v>
+        <v>345</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>22</v>
@@ -47417,12 +47741,12 @@
         <v>28</v>
       </c>
       <c r="G271" s="1" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>1922</v>
+        <v>377</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>22</v>
@@ -47431,7 +47755,7 @@
         <v>22</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E272" s="1" t="s">
         <v>22</v>
@@ -47440,12 +47764,12 @@
         <v>28</v>
       </c>
       <c r="G272" s="1" t="s">
-        <v>730</v>
+        <v>377</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
-        <v>603</v>
+        <v>1881</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>22</v>
@@ -47468,7 +47792,7 @@
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
-        <v>404</v>
+        <v>1922</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>22</v>
@@ -47477,7 +47801,7 @@
         <v>22</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E274" s="1" t="s">
         <v>22</v>
@@ -47486,12 +47810,12 @@
         <v>28</v>
       </c>
       <c r="G274" s="1" t="s">
-        <v>719</v>
+        <v>730</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A275" s="1" t="s">
-        <v>538</v>
+      <c r="A275" s="2" t="s">
+        <v>603</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>22</v>
@@ -47509,35 +47833,35 @@
         <v>28</v>
       </c>
       <c r="G275" s="1" t="s">
-        <v>732</v>
+        <v>720</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>338</v>
+        <v>404</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D276" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F276" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G276" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>414</v>
+        <v>538</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>22</v>
@@ -47546,7 +47870,7 @@
         <v>22</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E277" s="1" t="s">
         <v>22</v>
@@ -47555,12 +47879,12 @@
         <v>28</v>
       </c>
       <c r="G277" s="1" t="s">
-        <v>728</v>
+        <v>732</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278" s="1" t="s">
-        <v>517</v>
+      <c r="A278" s="2" t="s">
+        <v>338</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>22</v>
@@ -47583,7 +47907,7 @@
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>628</v>
+        <v>414</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>22</v>
@@ -47606,70 +47930,116 @@
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>595</v>
+        <v>517</v>
       </c>
       <c r="B280" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D280" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F280" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G280" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F281" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G281" s="1" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F282" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G282" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A283" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="B281" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C281" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D281" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E281" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F281" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G281" s="1" t="s">
+      <c r="B283" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F283" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G283" s="1" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A282" s="2" t="s">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A284" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B282" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C282" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D282" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E282" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F282" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G282" s="1" t="s">
+      <c r="B284" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F284" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G284" s="1" t="s">
         <v>720</v>
       </c>
     </row>
@@ -47681,10 +48051,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J978"/>
+  <dimension ref="A1:J983"/>
   <sheetViews>
-    <sheetView topLeftCell="A957" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A978" sqref="A978"/>
+    <sheetView topLeftCell="A962" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A983" sqref="A983"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62612,6 +62982,46 @@
       </c>
       <c r="B978" s="1" t="s">
         <v>1943</v>
+      </c>
+    </row>
+    <row r="979" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A979" s="1" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B979" s="1" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="980" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A980" s="1" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B980" s="1" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="981" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A981" s="1" t="s">
+        <v>1946</v>
+      </c>
+      <c r="B981" s="1" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="982" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A982" s="1" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B982" s="1" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="983" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A983" s="1" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B983" s="1" t="s">
+        <v>1952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ported fixes to CusCus recipes
</commit_message>
<xml_diff>
--- a/data_sources/scripts/files/FoodConnectsPeople.xlsx
+++ b/data_sources/scripts/files/FoodConnectsPeople.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Recipe" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14507" uniqueCount="2291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14508" uniqueCount="2291">
   <si>
     <t>id</t>
   </si>
@@ -7386,8 +7386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P141"/>
   <sheetViews>
-    <sheetView topLeftCell="D133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K141" sqref="K141"/>
+    <sheetView topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16438,8 +16438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1661"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A440" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B451" sqref="B451"/>
+    <sheetView topLeftCell="A1534" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1545" sqref="B1545"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39845,7 +39845,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="1473" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1473" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1473" s="1">
         <v>125</v>
       </c>
@@ -39853,7 +39853,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="1474" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1474" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1474" s="1">
         <v>125</v>
       </c>
@@ -39861,7 +39861,7 @@
         <v>2108</v>
       </c>
     </row>
-    <row r="1475" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1475" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1475" s="1">
         <v>125</v>
       </c>
@@ -39869,7 +39869,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="1476" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1476" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1476" s="1">
         <v>125</v>
       </c>
@@ -39877,7 +39877,7 @@
         <v>2105</v>
       </c>
     </row>
-    <row r="1477" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1477" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1477" s="1">
         <v>125</v>
       </c>
@@ -39885,7 +39885,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="1478" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1478" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1478" s="1">
         <v>125</v>
       </c>
@@ -39893,7 +39893,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="1479" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1479" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1479" s="1">
         <v>126</v>
       </c>
@@ -39907,7 +39907,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="1480" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1480" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1480" s="1">
         <v>126</v>
       </c>
@@ -39921,7 +39921,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="1481" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1481" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1481" s="1">
         <v>126</v>
       </c>
@@ -39935,7 +39935,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="1482" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1482" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1482" s="1">
         <v>126</v>
       </c>
@@ -39949,7 +39949,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="1483" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1483" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1483" s="1">
         <v>126</v>
       </c>
@@ -39962,8 +39962,11 @@
       <c r="D1483" s="1" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="1484" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1483" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1484" s="1">
         <v>126</v>
       </c>
@@ -39977,7 +39980,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="1485" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1485" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1485" s="1">
         <v>126</v>
       </c>
@@ -39991,7 +39994,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="1486" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1486" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1486" s="1">
         <v>126</v>
       </c>
@@ -40005,7 +40008,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="1487" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1487" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1487" s="1">
         <v>126</v>
       </c>
@@ -40019,7 +40022,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="1488" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1488" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1488" s="1">
         <v>126</v>
       </c>
@@ -40562,7 +40565,7 @@
         <v>2176</v>
       </c>
       <c r="C1531" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D1531" s="1" t="s">
         <v>365</v>
@@ -41029,10 +41032,10 @@
         <v>97</v>
       </c>
       <c r="C1568" s="1">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="D1568" s="1" t="s">
-        <v>470</v>
+        <v>373</v>
       </c>
     </row>
     <row r="1569" spans="1:4" x14ac:dyDescent="0.25">
@@ -41173,10 +41176,10 @@
         <v>97</v>
       </c>
       <c r="C1580" s="1">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="D1580" s="1" t="s">
-        <v>470</v>
+        <v>373</v>
       </c>
     </row>
     <row r="1581" spans="1:4" x14ac:dyDescent="0.25">
@@ -41451,7 +41454,7 @@
         <v>477</v>
       </c>
       <c r="C1602" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1602" s="1" t="s">
         <v>470</v>
@@ -41468,10 +41471,10 @@
         <v>97</v>
       </c>
       <c r="C1603" s="1">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="D1603" s="1" t="s">
-        <v>470</v>
+        <v>373</v>
       </c>
     </row>
     <row r="1604" spans="1:6" x14ac:dyDescent="0.25">
@@ -41482,10 +41485,10 @@
         <v>389</v>
       </c>
       <c r="C1604" s="1">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="D1604" s="1" t="s">
-        <v>470</v>
+        <v>373</v>
       </c>
     </row>
     <row r="1605" spans="1:6" x14ac:dyDescent="0.25">
@@ -41890,7 +41893,7 @@
         <v>506</v>
       </c>
       <c r="C1637" s="1">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="D1637" s="1" t="s">
         <v>373</v>
@@ -41918,7 +41921,7 @@
         <v>74</v>
       </c>
       <c r="C1639" s="1">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="D1639" s="1" t="s">
         <v>373</v>
@@ -41932,7 +41935,7 @@
         <v>68</v>
       </c>
       <c r="C1640" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1640" s="1" t="s">
         <v>365</v>
@@ -41946,7 +41949,7 @@
         <v>60</v>
       </c>
       <c r="C1641" s="1">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D1641" s="1" t="s">
         <v>373</v>
@@ -42212,8 +42215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F476"/>
   <sheetViews>
-    <sheetView topLeftCell="A402" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C415" sqref="C415"/>
+    <sheetView tabSelected="1" topLeftCell="A342" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A347" sqref="A347:XFD347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45978,58 +45981,55 @@
         <v>389</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>470</v>
+        <v>373</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D290">
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A291" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D291">
         <v>1000</v>
       </c>
-      <c r="E290" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A291" s="2" t="s">
+      <c r="E291" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A292" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B291" s="2" t="s">
+      <c r="B292" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C291" s="2" t="s">
+      <c r="C292" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="D291">
+      <c r="D292">
         <v>150</v>
       </c>
-      <c r="E291" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A292" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B292" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C292" s="1" t="s">
-        <v>365</v>
+      <c r="E292" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>561</v>
+        <v>296</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="D293">
-        <v>200</v>
+        <v>365</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -46037,37 +46037,40 @@
         <v>561</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>517</v>
+        <v>364</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>517</v>
       </c>
+      <c r="D294">
+        <v>200</v>
+      </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>365</v>
+        <v>517</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>365</v>
+        <v>517</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>586</v>
+        <v>562</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>517</v>
+        <v>365</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>517</v>
+        <v>365</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>616</v>
+        <v>586</v>
       </c>
       <c r="B297" s="1" t="s">
         <v>517</v>
@@ -46077,25 +46080,25 @@
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A298" s="2" t="s">
+      <c r="A298" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A299" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B298" s="2" t="s">
+      <c r="B299" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C298" s="2" t="s">
+      <c r="C299" s="2" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A299" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="B299" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="C299" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -46103,30 +46106,24 @@
         <v>628</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D300">
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A301" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D301">
         <v>20</v>
-      </c>
-      <c r="E300" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A301" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="B301" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="C301" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="D301">
-        <v>50</v>
       </c>
       <c r="E301" s="1" t="s">
         <v>28</v>
@@ -46137,13 +46134,13 @@
         <v>372</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>364</v>
+        <v>386</v>
       </c>
       <c r="C302" s="2" t="s">
         <v>373</v>
       </c>
       <c r="D302">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E302" s="1" t="s">
         <v>28</v>
@@ -46154,10 +46151,16 @@
         <v>372</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="C303" s="2" t="s">
         <v>373</v>
+      </c>
+      <c r="D303">
+        <v>30</v>
+      </c>
+      <c r="E303" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -46165,30 +46168,24 @@
         <v>372</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C304" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="D304">
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A305" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="D305">
         <v>10</v>
-      </c>
-      <c r="E304" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A305" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="B305" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="C305" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="D305">
-        <v>30</v>
       </c>
       <c r="E305" s="1" t="s">
         <v>28</v>
@@ -46198,110 +46195,116 @@
       <c r="A306" s="1" t="s">
         <v>372</v>
       </c>
+      <c r="B306" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D306">
+        <v>30</v>
+      </c>
+      <c r="E306" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="B307" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C307" s="1" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>422</v>
+        <v>365</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="D308">
-        <v>200</v>
-      </c>
-      <c r="E308" s="1" t="s">
-        <v>28</v>
+        <v>365</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>2114</v>
+        <v>644</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>470</v>
+        <v>422</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>373</v>
       </c>
       <c r="D309">
-        <v>1000</v>
-      </c>
-      <c r="E309" s="1"/>
+        <v>200</v>
+      </c>
+      <c r="E309" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>2285</v>
+        <v>2114</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>517</v>
+        <v>470</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>517</v>
+        <v>373</v>
+      </c>
+      <c r="D310">
+        <v>1000</v>
       </c>
       <c r="E310" s="1"/>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>611</v>
+        <v>2285</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>377</v>
+        <v>517</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>377</v>
-      </c>
+        <v>517</v>
+      </c>
+      <c r="E311" s="1"/>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
-        <v>2261</v>
+        <v>611</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>646</v>
+        <v>2261</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="D313">
-        <v>200</v>
-      </c>
-      <c r="E313" s="1" t="s">
-        <v>28</v>
+        <v>364</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>503</v>
+        <v>646</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>373</v>
+      </c>
+      <c r="D314">
+        <v>200</v>
+      </c>
+      <c r="E314" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
@@ -46309,77 +46312,77 @@
         <v>503</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>504</v>
+        <v>373</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>504</v>
+        <v>373</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>2059</v>
+        <v>503</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>373</v>
+        <v>504</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>373</v>
+        <v>504</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>2075</v>
+        <v>2059</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>576</v>
+        <v>373</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D317">
-        <v>350</v>
-      </c>
-      <c r="E317" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>551</v>
+        <v>2075</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>365</v>
+        <v>576</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>365</v>
+        <v>373</v>
+      </c>
+      <c r="D318">
+        <v>350</v>
+      </c>
+      <c r="E318" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>1228</v>
+        <v>551</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="D319">
-        <v>5</v>
-      </c>
-      <c r="E319" s="1" t="s">
-        <v>28</v>
+        <v>365</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>554</v>
+        <v>1228</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>373</v>
+      </c>
+      <c r="D320">
+        <v>5</v>
+      </c>
+      <c r="E320" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
@@ -46387,170 +46390,170 @@
         <v>554</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D321">
-        <v>20</v>
-      </c>
-      <c r="E321" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>491</v>
+        <v>554</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>368</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>368</v>
+        <v>373</v>
+      </c>
+      <c r="D322">
+        <v>20</v>
+      </c>
+      <c r="E322" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>2176</v>
+        <v>491</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>496</v>
+        <v>2176</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A326" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="B325" s="1" t="s">
+      <c r="B326" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="C325" s="1" t="s">
+      <c r="C326" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A326" s="2" t="s">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A327" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B326" s="2" t="s">
+      <c r="B327" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="C326" s="2" t="s">
+      <c r="C327" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="D326">
+      <c r="D327">
         <v>30</v>
       </c>
-      <c r="E326" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A327" s="1" t="s">
+      <c r="E327" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A328" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B327" s="1" t="s">
+      <c r="B328" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="C327" s="1" t="s">
+      <c r="C328" s="1" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A328" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B328" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="C328" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="D328">
-        <v>1000</v>
-      </c>
-      <c r="E328" s="1"/>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>365</v>
+        <v>470</v>
       </c>
       <c r="C329" s="2" t="s">
         <v>373</v>
       </c>
       <c r="D329">
+        <v>1000</v>
+      </c>
+      <c r="E329" s="1"/>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A330" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="D330">
         <v>200</v>
       </c>
-      <c r="E329" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A330" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B330" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C330" s="1" t="s">
-        <v>365</v>
+      <c r="E330" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>647</v>
+        <v>142</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>2038</v>
+        <v>647</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>373</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="D332">
-        <v>1</v>
-      </c>
-      <c r="E332" s="1" t="s">
-        <v>22</v>
+        <v>373</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>544</v>
+        <v>2038</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>373</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>373</v>
+        <v>517</v>
+      </c>
+      <c r="D333">
+        <v>1</v>
+      </c>
+      <c r="E333" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -46558,93 +46561,93 @@
         <v>544</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C334" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D334">
-        <v>10</v>
-      </c>
-      <c r="E334" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>493</v>
+        <v>544</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D335">
+        <v>10</v>
+      </c>
+      <c r="E335" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="B336" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C336" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="D336">
-        <v>10</v>
-      </c>
-      <c r="E336" s="1" t="s">
-        <v>28</v>
+        <v>493</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>404</v>
+        <v>696</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>365</v>
+        <v>377</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>365</v>
+        <v>373</v>
+      </c>
+      <c r="D337">
+        <v>10</v>
+      </c>
+      <c r="E337" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>2083</v>
+        <v>404</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="D338">
-        <v>100</v>
-      </c>
-      <c r="E338" s="1" t="s">
-        <v>28</v>
+        <v>365</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
+        <v>2083</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D339">
+        <v>100</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="B339" s="1" t="s">
+      <c r="B340" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="C339" s="1" t="s">
+      <c r="C340" s="1" t="s">
         <v>470</v>
-      </c>
-    </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A340" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="B340" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="C340" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
-        <v>445</v>
+        <v>399</v>
       </c>
       <c r="B341" s="2" t="s">
         <v>365</v>
@@ -46655,13 +46658,13 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
-        <v>643</v>
+        <v>445</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>517</v>
+        <v>365</v>
       </c>
       <c r="C342" s="2" t="s">
-        <v>517</v>
+        <v>365</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
@@ -46669,46 +46672,40 @@
         <v>643</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>364</v>
+        <v>517</v>
       </c>
       <c r="C343" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="D343">
-        <v>200</v>
-      </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>2048</v>
+        <v>643</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C344" s="2" t="s">
         <v>517</v>
       </c>
       <c r="D344">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A345" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="B345" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C345" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="D345">
         <v>30</v>
       </c>
-      <c r="E344" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A345" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B345" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C345" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="D345">
-        <v>200</v>
-      </c>
-      <c r="E345" s="1" t="s">
+      <c r="E345" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -46717,15 +46714,17 @@
         <v>97</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>470</v>
+        <v>364</v>
       </c>
       <c r="C346" s="1" t="s">
         <v>373</v>
       </c>
       <c r="D346">
-        <v>1000</v>
-      </c>
-      <c r="E346" s="1"/>
+        <v>200</v>
+      </c>
+      <c r="E346" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">

</xml_diff>

<commit_message>
Fix in swiched columns
</commit_message>
<xml_diff>
--- a/data_sources/scripts/files/FoodConnectsPeople.xlsx
+++ b/data_sources/scripts/files/FoodConnectsPeople.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="Recipe" sheetId="1" r:id="rId1"/>
@@ -7749,8 +7749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView topLeftCell="D134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K154" sqref="K154"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14346,10 +14346,10 @@
         <v>2361</v>
       </c>
       <c r="D150" s="1">
+        <v>60</v>
+      </c>
+      <c r="E150" s="1">
         <v>4</v>
-      </c>
-      <c r="E150" s="1">
-        <v>60</v>
       </c>
       <c r="F150" s="1">
         <v>3</v>
@@ -14390,10 +14390,10 @@
         <v>2375</v>
       </c>
       <c r="D151" s="1">
+        <v>120</v>
+      </c>
+      <c r="E151" s="1">
         <v>4</v>
-      </c>
-      <c r="E151" s="1">
-        <v>120</v>
       </c>
       <c r="F151" s="1">
         <v>3</v>
@@ -14434,10 +14434,10 @@
         <v>2374</v>
       </c>
       <c r="D152" s="1">
+        <v>180</v>
+      </c>
+      <c r="E152" s="1">
         <v>4</v>
-      </c>
-      <c r="E152" s="1">
-        <v>180</v>
       </c>
       <c r="F152" s="1">
         <v>4</v>
@@ -14478,10 +14478,10 @@
         <v>2381</v>
       </c>
       <c r="D153" s="1">
+        <v>180</v>
+      </c>
+      <c r="E153" s="1">
         <v>5</v>
-      </c>
-      <c r="E153" s="1">
-        <v>180</v>
       </c>
       <c r="F153" s="1">
         <v>2</v>
@@ -14522,10 +14522,10 @@
         <v>2401</v>
       </c>
       <c r="D154" s="1">
+        <v>180</v>
+      </c>
+      <c r="E154" s="1">
         <v>20</v>
-      </c>
-      <c r="E154" s="1">
-        <v>180</v>
       </c>
       <c r="F154" s="1">
         <v>3</v>
@@ -46044,7 +46044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FIxes to recipe 14 of CusCus II ws
</commit_message>
<xml_diff>
--- a/data_sources/scripts/files/FoodConnectsPeople.xlsx
+++ b/data_sources/scripts/files/FoodConnectsPeople.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15421" uniqueCount="2428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15423" uniqueCount="2428">
   <si>
     <t>id</t>
   </si>
@@ -17760,10 +17760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1819"/>
+  <dimension ref="A1:G1820"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1716" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1724" sqref="C1724"/>
+      <selection activeCell="D1725" sqref="D1725"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47113,7 +47113,7 @@
         <v>695</v>
       </c>
       <c r="C1722" s="4">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="D1722" s="4" t="s">
         <v>649</v>
@@ -47128,7 +47128,7 @@
         <v>813</v>
       </c>
       <c r="C1723" s="4">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D1723" s="4" t="s">
         <v>649</v>
@@ -47143,7 +47143,7 @@
         <v>175</v>
       </c>
       <c r="C1724" s="4">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D1724" s="4" t="s">
         <v>505</v>
@@ -47160,7 +47160,7 @@
         <v>712</v>
       </c>
       <c r="C1725" s="4">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="D1725" s="4" t="s">
         <v>497</v>
@@ -47169,7 +47169,7 @@
       <c r="F1725" s="4"/>
       <c r="G1725" s="5"/>
     </row>
-    <row r="1726" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1726" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1726" s="4">
         <v>148</v>
       </c>
@@ -47177,24 +47177,26 @@
         <v>592</v>
       </c>
       <c r="C1726" s="4">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D1726" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="E1726" s="5"/>
       <c r="F1726" s="4"/>
-      <c r="G1726" s="5"/>
     </row>
     <row r="1727" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1727" s="4">
         <v>148</v>
       </c>
       <c r="B1727" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="C1727" s="5"/>
-      <c r="D1727" s="5"/>
+        <v>592</v>
+      </c>
+      <c r="C1727" s="4">
+        <v>1</v>
+      </c>
+      <c r="D1727" s="4" t="s">
+        <v>500</v>
+      </c>
       <c r="E1727" s="5"/>
       <c r="F1727" s="4"/>
       <c r="G1727" s="5"/>
@@ -47204,7 +47206,7 @@
         <v>148</v>
       </c>
       <c r="B1728" s="4" t="s">
-        <v>530</v>
+        <v>507</v>
       </c>
       <c r="C1728" s="5"/>
       <c r="D1728" s="5"/>
@@ -47217,17 +47219,11 @@
         <v>148</v>
       </c>
       <c r="B1729" s="4" t="s">
-        <v>759</v>
-      </c>
-      <c r="C1729" s="4">
-        <v>100</v>
-      </c>
-      <c r="D1729" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="E1729" s="4" t="s">
-        <v>584</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="C1729" s="5"/>
+      <c r="D1729" s="5"/>
+      <c r="E1729" s="5"/>
       <c r="F1729" s="4"/>
       <c r="G1729" s="5"/>
     </row>
@@ -47236,11 +47232,17 @@
         <v>148</v>
       </c>
       <c r="B1730" s="4" t="s">
-        <v>568</v>
-      </c>
-      <c r="C1730" s="5"/>
-      <c r="D1730" s="5"/>
-      <c r="E1730" s="5"/>
+        <v>759</v>
+      </c>
+      <c r="C1730" s="4">
+        <v>50</v>
+      </c>
+      <c r="D1730" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="E1730" s="4" t="s">
+        <v>584</v>
+      </c>
       <c r="F1730" s="4"/>
       <c r="G1730" s="5"/>
     </row>
@@ -47249,17 +47251,11 @@
         <v>148</v>
       </c>
       <c r="B1731" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1731" s="4">
-        <v>100</v>
-      </c>
-      <c r="D1731" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="E1731" s="4" t="s">
-        <v>503</v>
-      </c>
+        <v>568</v>
+      </c>
+      <c r="C1731" s="5"/>
+      <c r="D1731" s="5"/>
+      <c r="E1731" s="5"/>
       <c r="F1731" s="4"/>
       <c r="G1731" s="5"/>
     </row>
@@ -47268,7 +47264,7 @@
         <v>148</v>
       </c>
       <c r="B1732" s="4" t="s">
-        <v>468</v>
+        <v>60</v>
       </c>
       <c r="C1732" s="4">
         <v>300</v>
@@ -47276,22 +47272,24 @@
       <c r="D1732" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="E1732" s="5"/>
+      <c r="E1732" s="4" t="s">
+        <v>503</v>
+      </c>
       <c r="F1732" s="4"/>
       <c r="G1732" s="5"/>
     </row>
     <row r="1733" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1733" s="4">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B1733" s="4" t="s">
-        <v>34</v>
+        <v>468</v>
       </c>
       <c r="C1733" s="4">
-        <v>2</v>
+        <v>600</v>
       </c>
       <c r="D1733" s="4" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="E1733" s="5"/>
       <c r="F1733" s="4"/>
@@ -47302,10 +47300,10 @@
         <v>149</v>
       </c>
       <c r="B1734" s="4" t="s">
-        <v>531</v>
+        <v>34</v>
       </c>
       <c r="C1734" s="4">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="D1734" s="4" t="s">
         <v>497</v>
@@ -47319,13 +47317,13 @@
         <v>149</v>
       </c>
       <c r="B1735" s="4" t="s">
-        <v>499</v>
+        <v>531</v>
       </c>
       <c r="C1735" s="4">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="D1735" s="4" t="s">
-        <v>649</v>
+        <v>497</v>
       </c>
       <c r="E1735" s="5"/>
       <c r="F1735" s="4"/>
@@ -47336,13 +47334,13 @@
         <v>149</v>
       </c>
       <c r="B1736" s="4" t="s">
-        <v>691</v>
+        <v>499</v>
       </c>
       <c r="C1736" s="4">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="D1736" s="4" t="s">
-        <v>505</v>
+        <v>649</v>
       </c>
       <c r="E1736" s="5"/>
       <c r="F1736" s="4"/>
@@ -47353,13 +47351,13 @@
         <v>149</v>
       </c>
       <c r="B1737" s="4" t="s">
-        <v>909</v>
+        <v>691</v>
       </c>
       <c r="C1737" s="4">
-        <v>0.5</v>
+        <v>300</v>
       </c>
       <c r="D1737" s="4" t="s">
-        <v>771</v>
+        <v>505</v>
       </c>
       <c r="E1737" s="5"/>
       <c r="F1737" s="4"/>
@@ -47370,13 +47368,13 @@
         <v>149</v>
       </c>
       <c r="B1738" s="4" t="s">
-        <v>759</v>
+        <v>909</v>
       </c>
       <c r="C1738" s="4">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="D1738" s="4" t="s">
-        <v>505</v>
+        <v>771</v>
       </c>
       <c r="E1738" s="5"/>
       <c r="F1738" s="4"/>
@@ -47387,13 +47385,13 @@
         <v>149</v>
       </c>
       <c r="B1739" s="4" t="s">
-        <v>507</v>
+        <v>759</v>
       </c>
       <c r="C1739" s="4">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D1739" s="4" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="E1739" s="5"/>
       <c r="F1739" s="4"/>
@@ -47404,13 +47402,13 @@
         <v>149</v>
       </c>
       <c r="B1740" s="4" t="s">
-        <v>797</v>
+        <v>507</v>
       </c>
       <c r="C1740" s="4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D1740" s="4" t="s">
-        <v>649</v>
+        <v>509</v>
       </c>
       <c r="E1740" s="5"/>
       <c r="F1740" s="4"/>
@@ -47421,13 +47419,13 @@
         <v>149</v>
       </c>
       <c r="B1741" s="4" t="s">
-        <v>549</v>
+        <v>797</v>
       </c>
       <c r="C1741" s="4">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D1741" s="4" t="s">
-        <v>497</v>
+        <v>649</v>
       </c>
       <c r="E1741" s="5"/>
       <c r="F1741" s="4"/>
@@ -47438,13 +47436,13 @@
         <v>149</v>
       </c>
       <c r="B1742" s="4" t="s">
-        <v>761</v>
+        <v>549</v>
       </c>
       <c r="C1742" s="4">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="D1742" s="4" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="E1742" s="5"/>
       <c r="F1742" s="4"/>
@@ -47455,13 +47453,13 @@
         <v>149</v>
       </c>
       <c r="B1743" s="4" t="s">
-        <v>521</v>
+        <v>761</v>
       </c>
       <c r="C1743" s="4">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="D1743" s="4" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="E1743" s="5"/>
       <c r="F1743" s="4"/>
@@ -47472,7 +47470,7 @@
         <v>149</v>
       </c>
       <c r="B1744" s="4" t="s">
-        <v>104</v>
+        <v>521</v>
       </c>
       <c r="C1744" s="4">
         <v>1</v>
@@ -47489,7 +47487,7 @@
         <v>149</v>
       </c>
       <c r="B1745" s="4" t="s">
-        <v>2426</v>
+        <v>104</v>
       </c>
       <c r="C1745" s="4">
         <v>1</v>
@@ -47506,13 +47504,13 @@
         <v>149</v>
       </c>
       <c r="B1746" s="4" t="s">
-        <v>701</v>
+        <v>2426</v>
       </c>
       <c r="C1746" s="4">
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="D1746" s="4" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="E1746" s="5"/>
       <c r="F1746" s="4"/>
@@ -47523,13 +47521,13 @@
         <v>149</v>
       </c>
       <c r="B1747" s="4" t="s">
-        <v>741</v>
+        <v>701</v>
       </c>
       <c r="C1747" s="4">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D1747" s="4" t="s">
-        <v>649</v>
+        <v>505</v>
       </c>
       <c r="E1747" s="5"/>
       <c r="F1747" s="4"/>
@@ -47540,10 +47538,10 @@
         <v>149</v>
       </c>
       <c r="B1748" s="4" t="s">
-        <v>499</v>
+        <v>741</v>
       </c>
       <c r="C1748" s="4">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="D1748" s="4" t="s">
         <v>649</v>
@@ -47557,10 +47555,14 @@
         <v>149</v>
       </c>
       <c r="B1749" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="C1749" s="5"/>
-      <c r="D1749" s="5"/>
+        <v>499</v>
+      </c>
+      <c r="C1749" s="4">
+        <v>50</v>
+      </c>
+      <c r="D1749" s="4" t="s">
+        <v>649</v>
+      </c>
       <c r="E1749" s="5"/>
       <c r="F1749" s="4"/>
       <c r="G1749" s="5"/>
@@ -47570,7 +47572,7 @@
         <v>149</v>
       </c>
       <c r="B1750" s="4" t="s">
-        <v>530</v>
+        <v>555</v>
       </c>
       <c r="C1750" s="5"/>
       <c r="D1750" s="5"/>
@@ -47583,7 +47585,7 @@
         <v>149</v>
       </c>
       <c r="B1751" s="4" t="s">
-        <v>514</v>
+        <v>530</v>
       </c>
       <c r="C1751" s="5"/>
       <c r="D1751" s="5"/>
@@ -47593,17 +47595,13 @@
     </row>
     <row r="1752" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1752" s="4">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1752" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1752" s="4">
-        <v>250</v>
-      </c>
-      <c r="D1752" s="4" t="s">
-        <v>505</v>
-      </c>
+        <v>514</v>
+      </c>
+      <c r="C1752" s="5"/>
+      <c r="D1752" s="5"/>
       <c r="E1752" s="5"/>
       <c r="F1752" s="4"/>
       <c r="G1752" s="5"/>
@@ -47613,7 +47611,7 @@
         <v>150</v>
       </c>
       <c r="B1753" s="4" t="s">
-        <v>691</v>
+        <v>60</v>
       </c>
       <c r="C1753" s="4">
         <v>250</v>
@@ -47630,13 +47628,13 @@
         <v>150</v>
       </c>
       <c r="B1754" s="4" t="s">
-        <v>549</v>
+        <v>691</v>
       </c>
       <c r="C1754" s="4">
-        <v>3</v>
+        <v>250</v>
       </c>
       <c r="D1754" s="4" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="E1754" s="5"/>
       <c r="F1754" s="4"/>
@@ -47647,13 +47645,13 @@
         <v>150</v>
       </c>
       <c r="B1755" s="4" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="C1755" s="4">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="D1755" s="4" t="s">
-        <v>649</v>
+        <v>497</v>
       </c>
       <c r="E1755" s="5"/>
       <c r="F1755" s="4"/>
@@ -47664,10 +47662,14 @@
         <v>150</v>
       </c>
       <c r="B1756" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="C1756" s="5"/>
-      <c r="D1756" s="5"/>
+        <v>555</v>
+      </c>
+      <c r="C1756" s="4">
+        <v>100</v>
+      </c>
+      <c r="D1756" s="4" t="s">
+        <v>649</v>
+      </c>
       <c r="E1756" s="5"/>
       <c r="F1756" s="4"/>
       <c r="G1756" s="5"/>
@@ -47677,7 +47679,7 @@
         <v>150</v>
       </c>
       <c r="B1757" s="4" t="s">
-        <v>568</v>
+        <v>507</v>
       </c>
       <c r="C1757" s="5"/>
       <c r="D1757" s="5"/>
@@ -47690,17 +47692,11 @@
         <v>150</v>
       </c>
       <c r="B1758" s="4" t="s">
-        <v>780</v>
-      </c>
-      <c r="C1758" s="4">
-        <v>100</v>
-      </c>
-      <c r="D1758" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="E1758" s="4" t="s">
-        <v>762</v>
-      </c>
+        <v>568</v>
+      </c>
+      <c r="C1758" s="5"/>
+      <c r="D1758" s="5"/>
+      <c r="E1758" s="5"/>
       <c r="F1758" s="4"/>
       <c r="G1758" s="5"/>
     </row>
@@ -47709,15 +47705,17 @@
         <v>150</v>
       </c>
       <c r="B1759" s="4" t="s">
-        <v>813</v>
+        <v>780</v>
       </c>
       <c r="C1759" s="4">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D1759" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="E1759" s="5"/>
+      <c r="E1759" s="4" t="s">
+        <v>762</v>
+      </c>
       <c r="F1759" s="4"/>
       <c r="G1759" s="5"/>
     </row>
@@ -47726,10 +47724,10 @@
         <v>150</v>
       </c>
       <c r="B1760" s="4" t="s">
-        <v>465</v>
+        <v>813</v>
       </c>
       <c r="C1760" s="4">
-        <v>30</v>
+        <v>250</v>
       </c>
       <c r="D1760" s="4" t="s">
         <v>505</v>
@@ -47743,10 +47741,14 @@
         <v>150</v>
       </c>
       <c r="B1761" s="4" t="s">
-        <v>530</v>
-      </c>
-      <c r="C1761" s="5"/>
-      <c r="D1761" s="5"/>
+        <v>465</v>
+      </c>
+      <c r="C1761" s="4">
+        <v>30</v>
+      </c>
+      <c r="D1761" s="4" t="s">
+        <v>505</v>
+      </c>
       <c r="E1761" s="5"/>
       <c r="F1761" s="4"/>
       <c r="G1761" s="5"/>
@@ -47756,7 +47758,7 @@
         <v>150</v>
       </c>
       <c r="B1762" s="4" t="s">
-        <v>507</v>
+        <v>530</v>
       </c>
       <c r="C1762" s="5"/>
       <c r="D1762" s="5"/>
@@ -47769,34 +47771,28 @@
         <v>150</v>
       </c>
       <c r="B1763" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="C1763" s="4">
-        <v>3</v>
-      </c>
-      <c r="D1763" s="4" t="s">
-        <v>505</v>
-      </c>
+        <v>507</v>
+      </c>
+      <c r="C1763" s="5"/>
+      <c r="D1763" s="5"/>
       <c r="E1763" s="5"/>
       <c r="F1763" s="4"/>
       <c r="G1763" s="5"/>
     </row>
     <row r="1764" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1764" s="4">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1764" s="4" t="s">
-        <v>201</v>
+        <v>613</v>
       </c>
       <c r="C1764" s="4">
-        <v>400</v>
+        <v>3</v>
       </c>
       <c r="D1764" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="E1764" s="4" t="s">
-        <v>597</v>
-      </c>
+      <c r="E1764" s="5"/>
       <c r="F1764" s="4"/>
       <c r="G1764" s="5"/>
     </row>
@@ -47805,15 +47801,17 @@
         <v>151</v>
       </c>
       <c r="B1765" s="4" t="s">
-        <v>60</v>
+        <v>201</v>
       </c>
       <c r="C1765" s="4">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="D1765" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="E1765" s="5"/>
+      <c r="E1765" s="4" t="s">
+        <v>597</v>
+      </c>
       <c r="F1765" s="4"/>
       <c r="G1765" s="5"/>
     </row>
@@ -47822,10 +47820,10 @@
         <v>151</v>
       </c>
       <c r="B1766" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="C1766" s="4">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D1766" s="4" t="s">
         <v>505</v>
@@ -47839,10 +47837,10 @@
         <v>151</v>
       </c>
       <c r="B1767" s="4" t="s">
-        <v>759</v>
+        <v>97</v>
       </c>
       <c r="C1767" s="4">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D1767" s="4" t="s">
         <v>505</v>
@@ -47856,13 +47854,13 @@
         <v>151</v>
       </c>
       <c r="B1768" s="4" t="s">
-        <v>549</v>
+        <v>759</v>
       </c>
       <c r="C1768" s="4">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="D1768" s="4" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="E1768" s="5"/>
       <c r="F1768" s="4"/>
@@ -47873,10 +47871,14 @@
         <v>151</v>
       </c>
       <c r="B1769" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="C1769" s="5"/>
-      <c r="D1769" s="5"/>
+        <v>549</v>
+      </c>
+      <c r="C1769" s="4">
+        <v>1</v>
+      </c>
+      <c r="D1769" s="4" t="s">
+        <v>497</v>
+      </c>
       <c r="E1769" s="5"/>
       <c r="F1769" s="4"/>
       <c r="G1769" s="5"/>
@@ -47886,7 +47888,7 @@
         <v>151</v>
       </c>
       <c r="B1770" s="4" t="s">
-        <v>530</v>
+        <v>507</v>
       </c>
       <c r="C1770" s="5"/>
       <c r="D1770" s="5"/>
@@ -47899,14 +47901,10 @@
         <v>151</v>
       </c>
       <c r="B1771" s="4" t="s">
-        <v>691</v>
-      </c>
-      <c r="C1771" s="4">
-        <v>400</v>
-      </c>
-      <c r="D1771" s="4" t="s">
-        <v>505</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="C1771" s="5"/>
+      <c r="D1771" s="5"/>
       <c r="E1771" s="5"/>
       <c r="F1771" s="4"/>
       <c r="G1771" s="5"/>
@@ -47916,10 +47914,10 @@
         <v>151</v>
       </c>
       <c r="B1772" s="4" t="s">
-        <v>748</v>
+        <v>691</v>
       </c>
       <c r="C1772" s="4">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="D1772" s="4" t="s">
         <v>505</v>
@@ -47933,13 +47931,13 @@
         <v>151</v>
       </c>
       <c r="B1773" s="4" t="s">
-        <v>549</v>
+        <v>748</v>
       </c>
       <c r="C1773" s="4">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D1773" s="4" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="E1773" s="5"/>
       <c r="F1773" s="4"/>
@@ -47950,13 +47948,13 @@
         <v>151</v>
       </c>
       <c r="B1774" s="4" t="s">
-        <v>465</v>
+        <v>549</v>
       </c>
       <c r="C1774" s="4">
-        <v>250</v>
+        <v>5</v>
       </c>
       <c r="D1774" s="4" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="E1774" s="5"/>
       <c r="F1774" s="4"/>
@@ -47967,13 +47965,13 @@
         <v>151</v>
       </c>
       <c r="B1775" s="4" t="s">
-        <v>818</v>
+        <v>465</v>
       </c>
       <c r="C1775" s="4">
-        <v>2</v>
+        <v>250</v>
       </c>
       <c r="D1775" s="4" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="E1775" s="5"/>
       <c r="F1775" s="4"/>
@@ -47984,13 +47982,13 @@
         <v>151</v>
       </c>
       <c r="B1776" s="4" t="s">
-        <v>811</v>
+        <v>818</v>
       </c>
       <c r="C1776" s="4">
         <v>2</v>
       </c>
       <c r="D1776" s="4" t="s">
-        <v>558</v>
+        <v>497</v>
       </c>
       <c r="E1776" s="5"/>
       <c r="F1776" s="4"/>
@@ -47998,16 +47996,16 @@
     </row>
     <row r="1777" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1777" s="4">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1777" s="4" t="s">
-        <v>691</v>
+        <v>811</v>
       </c>
       <c r="C1777" s="4">
-        <v>500</v>
+        <v>2</v>
       </c>
       <c r="D1777" s="4" t="s">
-        <v>505</v>
+        <v>558</v>
       </c>
       <c r="E1777" s="5"/>
       <c r="F1777" s="4"/>
@@ -48018,10 +48016,10 @@
         <v>152</v>
       </c>
       <c r="B1778" s="4" t="s">
-        <v>748</v>
+        <v>691</v>
       </c>
       <c r="C1778" s="4">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D1778" s="4" t="s">
         <v>505</v>
@@ -48035,10 +48033,10 @@
         <v>152</v>
       </c>
       <c r="B1779" s="4" t="s">
-        <v>910</v>
+        <v>748</v>
       </c>
       <c r="C1779" s="4">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="D1779" s="4" t="s">
         <v>505</v>
@@ -48052,13 +48050,13 @@
         <v>152</v>
       </c>
       <c r="B1780" s="4" t="s">
-        <v>508</v>
+        <v>910</v>
       </c>
       <c r="C1780" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D1780" s="4" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="E1780" s="5"/>
       <c r="F1780" s="4"/>
@@ -48069,7 +48067,7 @@
         <v>152</v>
       </c>
       <c r="B1781" s="4" t="s">
-        <v>499</v>
+        <v>508</v>
       </c>
       <c r="C1781" s="4">
         <v>1</v>
@@ -48086,10 +48084,10 @@
         <v>152</v>
       </c>
       <c r="B1782" s="4" t="s">
-        <v>695</v>
+        <v>499</v>
       </c>
       <c r="C1782" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1782" s="4" t="s">
         <v>500</v>
@@ -48103,10 +48101,14 @@
         <v>152</v>
       </c>
       <c r="B1783" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="C1783" s="5"/>
-      <c r="D1783" s="5"/>
+        <v>695</v>
+      </c>
+      <c r="C1783" s="4">
+        <v>2</v>
+      </c>
+      <c r="D1783" s="4" t="s">
+        <v>500</v>
+      </c>
       <c r="E1783" s="5"/>
       <c r="F1783" s="4"/>
       <c r="G1783" s="5"/>
@@ -48116,14 +48118,10 @@
         <v>152</v>
       </c>
       <c r="B1784" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="C1784" s="4">
-        <v>500</v>
-      </c>
-      <c r="D1784" s="4" t="s">
-        <v>649</v>
-      </c>
+        <v>507</v>
+      </c>
+      <c r="C1784" s="5"/>
+      <c r="D1784" s="5"/>
       <c r="E1784" s="5"/>
       <c r="F1784" s="4"/>
       <c r="G1784" s="5"/>
@@ -48133,13 +48131,13 @@
         <v>152</v>
       </c>
       <c r="B1785" s="4" t="s">
-        <v>911</v>
+        <v>555</v>
       </c>
       <c r="C1785" s="4">
         <v>500</v>
       </c>
       <c r="D1785" s="4" t="s">
-        <v>505</v>
+        <v>649</v>
       </c>
       <c r="E1785" s="5"/>
       <c r="F1785" s="4"/>
@@ -48150,10 +48148,10 @@
         <v>152</v>
       </c>
       <c r="B1786" s="4" t="s">
-        <v>741</v>
+        <v>911</v>
       </c>
       <c r="C1786" s="4">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D1786" s="4" t="s">
         <v>505</v>
@@ -48167,10 +48165,10 @@
         <v>152</v>
       </c>
       <c r="B1787" s="4" t="s">
-        <v>912</v>
+        <v>741</v>
       </c>
       <c r="C1787" s="4">
-        <v>750</v>
+        <v>100</v>
       </c>
       <c r="D1787" s="4" t="s">
         <v>505</v>
@@ -48184,10 +48182,10 @@
         <v>152</v>
       </c>
       <c r="B1788" s="4" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C1788" s="4">
-        <v>30</v>
+        <v>750</v>
       </c>
       <c r="D1788" s="4" t="s">
         <v>505</v>
@@ -48201,10 +48199,10 @@
         <v>152</v>
       </c>
       <c r="B1789" s="4" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C1789" s="4">
-        <v>250</v>
+        <v>30</v>
       </c>
       <c r="D1789" s="4" t="s">
         <v>505</v>
@@ -48218,10 +48216,10 @@
         <v>152</v>
       </c>
       <c r="B1790" s="4" t="s">
-        <v>583</v>
+        <v>914</v>
       </c>
       <c r="C1790" s="4">
-        <v>20</v>
+        <v>250</v>
       </c>
       <c r="D1790" s="4" t="s">
         <v>505</v>
@@ -48235,10 +48233,14 @@
         <v>152</v>
       </c>
       <c r="B1791" s="4" t="s">
-        <v>684</v>
-      </c>
-      <c r="C1791" s="5"/>
-      <c r="D1791" s="5"/>
+        <v>583</v>
+      </c>
+      <c r="C1791" s="4">
+        <v>20</v>
+      </c>
+      <c r="D1791" s="4" t="s">
+        <v>505</v>
+      </c>
       <c r="E1791" s="5"/>
       <c r="F1791" s="4"/>
       <c r="G1791" s="5"/>
@@ -48248,7 +48250,7 @@
         <v>152</v>
       </c>
       <c r="B1792" s="4" t="s">
-        <v>499</v>
+        <v>684</v>
       </c>
       <c r="C1792" s="5"/>
       <c r="D1792" s="5"/>
@@ -48261,7 +48263,7 @@
         <v>152</v>
       </c>
       <c r="B1793" s="4" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="C1793" s="5"/>
       <c r="D1793" s="5"/>
@@ -48271,17 +48273,13 @@
     </row>
     <row r="1794" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1794" s="4">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B1794" s="4" t="s">
-        <v>546</v>
-      </c>
-      <c r="C1794" s="4">
-        <v>10</v>
-      </c>
-      <c r="D1794" s="4" t="s">
-        <v>915</v>
-      </c>
+        <v>507</v>
+      </c>
+      <c r="C1794" s="5"/>
+      <c r="D1794" s="5"/>
       <c r="E1794" s="5"/>
       <c r="F1794" s="4"/>
       <c r="G1794" s="5"/>
@@ -48291,13 +48289,13 @@
         <v>153</v>
       </c>
       <c r="B1795" s="4" t="s">
-        <v>916</v>
+        <v>546</v>
       </c>
       <c r="C1795" s="4">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="D1795" s="4" t="s">
-        <v>505</v>
+        <v>915</v>
       </c>
       <c r="E1795" s="5"/>
       <c r="F1795" s="4"/>
@@ -48308,13 +48306,13 @@
         <v>153</v>
       </c>
       <c r="B1796" s="4" t="s">
-        <v>521</v>
+        <v>916</v>
       </c>
       <c r="C1796" s="4">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D1796" s="4" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="E1796" s="5"/>
       <c r="F1796" s="4"/>
@@ -48325,13 +48323,13 @@
         <v>153</v>
       </c>
       <c r="B1797" s="4" t="s">
-        <v>55</v>
+        <v>521</v>
       </c>
       <c r="C1797" s="4">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="D1797" s="4" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="E1797" s="5"/>
       <c r="F1797" s="4"/>
@@ -48342,13 +48340,13 @@
         <v>153</v>
       </c>
       <c r="B1798" s="4" t="s">
-        <v>549</v>
+        <v>55</v>
       </c>
       <c r="C1798" s="4">
-        <v>4</v>
+        <v>250</v>
       </c>
       <c r="D1798" s="4" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="E1798" s="5"/>
       <c r="F1798" s="4"/>
@@ -48359,13 +48357,13 @@
         <v>153</v>
       </c>
       <c r="B1799" s="4" t="s">
-        <v>695</v>
+        <v>549</v>
       </c>
       <c r="C1799" s="4">
-        <v>500</v>
+        <v>4</v>
       </c>
       <c r="D1799" s="4" t="s">
-        <v>649</v>
+        <v>497</v>
       </c>
       <c r="E1799" s="5"/>
       <c r="F1799" s="4"/>
@@ -48376,13 +48374,13 @@
         <v>153</v>
       </c>
       <c r="B1800" s="4" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c r="C1800" s="4">
         <v>500</v>
       </c>
       <c r="D1800" s="4" t="s">
-        <v>505</v>
+        <v>649</v>
       </c>
       <c r="E1800" s="5"/>
       <c r="F1800" s="4"/>
@@ -48393,10 +48391,14 @@
         <v>153</v>
       </c>
       <c r="B1801" s="4" t="s">
-        <v>568</v>
-      </c>
-      <c r="C1801" s="5"/>
-      <c r="D1801" s="5"/>
+        <v>691</v>
+      </c>
+      <c r="C1801" s="4">
+        <v>500</v>
+      </c>
+      <c r="D1801" s="4" t="s">
+        <v>505</v>
+      </c>
       <c r="E1801" s="5"/>
       <c r="F1801" s="4"/>
       <c r="G1801" s="5"/>
@@ -48406,7 +48408,7 @@
         <v>153</v>
       </c>
       <c r="B1802" s="4" t="s">
-        <v>507</v>
+        <v>568</v>
       </c>
       <c r="C1802" s="5"/>
       <c r="D1802" s="5"/>
@@ -48419,7 +48421,7 @@
         <v>153</v>
       </c>
       <c r="B1803" s="4" t="s">
-        <v>530</v>
+        <v>507</v>
       </c>
       <c r="C1803" s="5"/>
       <c r="D1803" s="5"/>
@@ -48432,14 +48434,10 @@
         <v>153</v>
       </c>
       <c r="B1804" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="C1804" s="4">
-        <v>250</v>
-      </c>
-      <c r="D1804" s="4" t="s">
-        <v>505</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="C1804" s="5"/>
+      <c r="D1804" s="5"/>
       <c r="E1804" s="5"/>
       <c r="F1804" s="4"/>
       <c r="G1804" s="5"/>
@@ -48449,30 +48447,30 @@
         <v>153</v>
       </c>
       <c r="B1805" s="4" t="s">
-        <v>801</v>
-      </c>
-      <c r="C1805" s="4"/>
-      <c r="D1805" s="4"/>
-      <c r="E1805" s="4" t="s">
-        <v>584</v>
-      </c>
+        <v>465</v>
+      </c>
+      <c r="C1805" s="4">
+        <v>250</v>
+      </c>
+      <c r="D1805" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="E1805" s="5"/>
       <c r="F1805" s="4"/>
       <c r="G1805" s="5"/>
     </row>
     <row r="1806" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1806" s="4">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B1806" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1806" s="4">
-        <v>4</v>
-      </c>
-      <c r="D1806" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="E1806" s="4"/>
+        <v>801</v>
+      </c>
+      <c r="C1806" s="4"/>
+      <c r="D1806" s="4"/>
+      <c r="E1806" s="4" t="s">
+        <v>584</v>
+      </c>
       <c r="F1806" s="4"/>
       <c r="G1806" s="5"/>
     </row>
@@ -48481,7 +48479,7 @@
         <v>154</v>
       </c>
       <c r="B1807" s="4" t="s">
-        <v>34</v>
+        <v>175</v>
       </c>
       <c r="C1807" s="4">
         <v>4</v>
@@ -48498,10 +48496,14 @@
         <v>154</v>
       </c>
       <c r="B1808" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="C1808" s="4"/>
-      <c r="D1808" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="C1808" s="4">
+        <v>4</v>
+      </c>
+      <c r="D1808" s="4" t="s">
+        <v>497</v>
+      </c>
       <c r="E1808" s="4"/>
       <c r="F1808" s="4"/>
       <c r="G1808" s="5"/>
@@ -48511,7 +48513,7 @@
         <v>154</v>
       </c>
       <c r="B1809" s="4" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="C1809" s="4"/>
       <c r="D1809" s="4"/>
@@ -48524,7 +48526,7 @@
         <v>154</v>
       </c>
       <c r="B1810" s="4" t="s">
-        <v>530</v>
+        <v>507</v>
       </c>
       <c r="C1810" s="4"/>
       <c r="D1810" s="4"/>
@@ -48537,7 +48539,7 @@
         <v>154</v>
       </c>
       <c r="B1811" s="4" t="s">
-        <v>513</v>
+        <v>530</v>
       </c>
       <c r="C1811" s="4"/>
       <c r="D1811" s="4"/>
@@ -48547,17 +48549,13 @@
     </row>
     <row r="1812" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1812" s="4">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B1812" s="4" t="s">
-        <v>917</v>
-      </c>
-      <c r="C1812" s="4">
-        <v>500</v>
-      </c>
-      <c r="D1812" s="4" t="s">
-        <v>505</v>
-      </c>
+        <v>513</v>
+      </c>
+      <c r="C1812" s="4"/>
+      <c r="D1812" s="4"/>
       <c r="E1812" s="4"/>
       <c r="F1812" s="4"/>
       <c r="G1812" s="5"/>
@@ -48567,10 +48565,10 @@
         <v>155</v>
       </c>
       <c r="B1813" s="4" t="s">
-        <v>658</v>
+        <v>917</v>
       </c>
       <c r="C1813" s="4">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="D1813" s="4" t="s">
         <v>505</v>
@@ -48584,17 +48582,15 @@
         <v>155</v>
       </c>
       <c r="B1814" s="4" t="s">
-        <v>521</v>
+        <v>658</v>
       </c>
       <c r="C1814" s="4">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="D1814" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="E1814" s="4" t="s">
-        <v>762</v>
-      </c>
+        <v>505</v>
+      </c>
+      <c r="E1814" s="4"/>
       <c r="F1814" s="4"/>
       <c r="G1814" s="5"/>
     </row>
@@ -48603,16 +48599,16 @@
         <v>155</v>
       </c>
       <c r="B1815" s="4" t="s">
-        <v>761</v>
+        <v>521</v>
       </c>
       <c r="C1815" s="4">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="D1815" s="4" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="E1815" s="4" t="s">
-        <v>510</v>
+        <v>762</v>
       </c>
       <c r="F1815" s="4"/>
       <c r="G1815" s="5"/>
@@ -48622,11 +48618,17 @@
         <v>155</v>
       </c>
       <c r="B1816" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="C1816" s="4"/>
-      <c r="D1816" s="4"/>
-      <c r="E1816" s="4"/>
+        <v>761</v>
+      </c>
+      <c r="C1816" s="4">
+        <v>300</v>
+      </c>
+      <c r="D1816" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="E1816" s="4" t="s">
+        <v>510</v>
+      </c>
       <c r="F1816" s="4"/>
       <c r="G1816" s="5"/>
     </row>
@@ -48635,7 +48637,7 @@
         <v>155</v>
       </c>
       <c r="B1817" s="4" t="s">
-        <v>530</v>
+        <v>507</v>
       </c>
       <c r="C1817" s="4"/>
       <c r="D1817" s="4"/>
@@ -48648,7 +48650,7 @@
         <v>155</v>
       </c>
       <c r="B1818" s="4" t="s">
-        <v>499</v>
+        <v>530</v>
       </c>
       <c r="C1818" s="4"/>
       <c r="D1818" s="4"/>
@@ -48661,15 +48663,28 @@
         <v>155</v>
       </c>
       <c r="B1819" s="4" t="s">
-        <v>759</v>
+        <v>499</v>
       </c>
       <c r="C1819" s="4"/>
       <c r="D1819" s="4"/>
-      <c r="E1819" s="4" t="s">
-        <v>584</v>
-      </c>
+      <c r="E1819" s="4"/>
       <c r="F1819" s="4"/>
       <c r="G1819" s="5"/>
+    </row>
+    <row r="1820" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1820" s="4">
+        <v>155</v>
+      </c>
+      <c r="B1820" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="C1820" s="4"/>
+      <c r="D1820" s="4"/>
+      <c r="E1820" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="F1820" s="4"/>
+      <c r="G1820" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>